<commit_message>
feat: update project with latest changes (logging, cleanup)
</commit_message>
<xml_diff>
--- a/data/noticias_historico.xlsx
+++ b/data/noticias_historico.xlsx
@@ -458,8 +458,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaNoticias" displayName="TablaNoticias" ref="A1:H46" headerRowCount="1">
-  <autoFilter ref="A1:H46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaNoticias" displayName="TablaNoticias" ref="A1:H68" headerRowCount="1">
+  <autoFilter ref="A1:H68"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Nombre del periódico"/>
     <tableColumn id="2" name="Procedencia"/>
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>35</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -840,17 +840,17 @@
         </is>
       </c>
       <c r="C23" s="4" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>Política social</t>
+          <t>Economia</t>
         </is>
       </c>
       <c r="C24" s="4" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25">
@@ -860,27 +860,27 @@
         </is>
       </c>
       <c r="C25" s="4" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>Economia</t>
+          <t>Tecnología industrial</t>
         </is>
       </c>
       <c r="C26" s="4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>Tecnología industrial</t>
+          <t>Política social</t>
         </is>
       </c>
       <c r="C27" s="4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
@@ -925,41 +925,41 @@
     <row r="38">
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>Negativa</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="C38" s="4" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Negativa</t>
         </is>
       </c>
       <c r="C39" s="4" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Positiva</t>
+          <t>Muy positiva</t>
         </is>
       </c>
       <c r="C40" s="4" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Muy positiva</t>
+          <t>Positiva</t>
         </is>
       </c>
       <c r="C41" s="4" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42">
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="C42" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -984,7 +984,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3496,6 +3496,1117 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C47" s="5" t="inlineStr">
+        <is>
+          <t>Las exportaciones de Castilla-La Mancha de enero a octubre de 2025 sube un 6% respecto al mismo periodo del año anterior</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-12-22T19:04:36+01:00</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Las exportaciones de Castilla-La Mancha alcanzaron en el mes de octubre de 2025 la cifra de 9.359,3 millones de euros , lo que supone un aumento del 6,0% respecto a octubre de 2024 , mientras que en España subieron un 0,8% respecto al mismo periodo año anterior, situándose en 324.772,7 millones de euros, según el último informe elaborado por la Dirección Territorial de Comercio-ICEX en Castilla-La Mancha . Por provincias, Toledo ocupó la primera posición con 2.843,9 millones de euros (+12,4%). Guadalajara se sitúa en segundo lugar con 2.505,2 millones (+11,7%). Ciudad Real es la tercera provincia exportadora, con 2.015,2 millones (-2,4%), y le siguen las provincias de Albacete con 1.323,6 millones (+0,8%), y Cuenca con 671,3 millones de euros, que registra un descenso en la exportación del 1,4%. En cuanto a los sectores exportadores , de enero a octubre de 2025, los productos Agroalimentarios ocuparon la primera posición con 3.253 millones de euros, representando el 34,8% del total exportado por Castilla-La Mancha y registrando un aumento del 5,7% respecto al mismo periodo anterior. Las exportaciones de aceites y grasas bajaron un 9,6% (293,1 millones de euros). Respecto a los países de destino, la Unión Europea acaparó el grueso de las exportaciones de la región con el 75,7% del total, liderada por Portugal con 2.212,3 millones de euros (+9,2%), seguida de Francia con 1.414,1 millones (-2,9%) y Alemania con 945,1 millones de euros (-0,8%). Fuera de ella, Reino Unido se sitúa en 324,8 millones (-6,5%), Estados Unidos con 263,3 millones (-8,4%) o China con 257,8 millones de euros (+124,1%), entre otros. Por su parte, las importaciones de la región alcanzaron los 14.714,9 millones de euros , subiendo un 5,4%, mientras que en España subieron un 4,9% hasta los 370.572,1 millones de euros. Por provincias importadoras, Guadalajara se sitúa en primer lugar , con un aumento del 4,3%, seguida de Toledo (+12,3%), Albacete (+3,9%), Ciudad Real (-4,2%) y Cuenca (-24,1%). Dentro de los sectores importadores, los Bienes de Equipo destacan sobre el resto con 4.197,7 millones de euros (-4,4%), seguido de los Productos Químicos con 2.894,9 millones (+16,0%), y Alimentación, bebidas y tabaco con un valor de 2.533,2 millones de euros (+8,3%). En cuanto a los países de procedencia, el 70,7 % tienen origen comunitario (Alemania y Francia, principalmente). Fuera de la UE, cabe destacar el 11,2% de nuestro principal proveedor no comunitario que es China, con 1.644,4 millones, que subió un 36,2% respecto al periodo enero - octubre de 2024. El saldo comercial de la región hasta octubre de 2025 se situó en -5.355,6 millones de euros, mientras que la tasa de cobertura (Xs/Ms) se situó en el 63,6%, aun claramente inferior a la media nacional (87,6%).</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Fran Malara
+Toledo
+Esta funcionalidad es sólo para registrados
+Esta funcionalidad es sólo para registrados
+Las exportaciones de Castilla-La Mancha alcanzaron en el mes de octubre de 2025 la cifra de9.359,3 millones de euros, lo que supone unaumento del 6,0% respecto a octubre de 2024, mientras que en España subieron un 0,...8% respecto al mismo periodo año anterior, situándose en 324.772,7 millones de euros, según el último informe elaborado por laDirección Territorial de Comercio-ICEX en Castilla-La Mancha.
+Por provincias,Toledo ocupó la primera posicióncon 2.843,9 millones de euros (+12,4%). Guadalajara se sitúa en segundo lugar con 2.505,2 millones (+11,7%). Ciudad Real es la tercera provincia exportadora, con 2.015,2 millones (-2,4%), y le siguen las provincias de Albacete con 1.323,6 millones (+0,8%), y Cuenca con 671,3 millones de euros, que registra un descenso en la exportación del 1,4%.
+En cuanto a lossectores exportadores, de enero a octubre de 2025,los productos Agroalimentarios ocuparon la primera posicióncon 3.253 millones de euros, representando el 34,8% del total exportado por Castilla-La Mancha y registrando un aumento del 5,7% respecto al mismo periodo anterior. Las exportaciones de aceites y grasas bajaron un 9,6% (293,1 millones de euros).
+Respecto a los países de destino,la Unión Europea acaparó el grueso de las exportaciones de la regióncon el 75,7% del total, liderada por Portugal con 2.212,3 millones de euros (+9,2%), seguida de Francia con 1.414,1 millones (-2,9%) y Alemania con 945,1 millones de euros (-0,8%). Fuera de ella,Reino Unido se sitúa en 324,8 millones(-6,5%), Estados Unidos con 263,3 millones (-8,4%) o China con 257,8 millones de euros (+124,1%), entre otros.
+Por su parte, las importaciones de la regiónalcanzaron los14.714,9 millones de euros, subiendo un 5,4%, mientras que en España subieron un 4,9% hasta los 370.572,1 millones de euros.
+Por provincias importadoras,Guadalajara se sitúa en primer lugar, con un aumento del 4,3%, seguida de Toledo (+12,3%), Albacete (+3,9%), Ciudad Real (-4,2%) y Cuenca (-24,1%).
+Dentro de los sectores importadores,los Bienes de Equipo destacan sobre el resto  con 4.197,7 millones de euros(-4,4%), seguido de los Productos Químicos con 2.894,9 millones (+16,0%), y Alimentación, bebidas y tabaco con un valor de 2.533,2 millones de euros (+8,3%).
+En cuanto a los países de procedencia,el 70,7 % tienen origen comunitario(Alemania y Francia, principalmente). Fuera de la UE, cabe destacar el 11,2% de nuestro principal proveedor no comunitario que es China, con 1.644,4 millones, que subió un 36,2% respecto al periodo enero - octubre de 2024.
+Elsaldo comercial de la regiónhasta octubre de 2025 se situó en -5.355,6 millones de euros, mientras que latasa de cobertura(Xs/Ms) se situó en el 63,6%, aunclaramente inferior a la media nacional(87,6%).</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>La Vanguardia</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C48" s="5" t="inlineStr">
+        <is>
+          <t>Regalar Dockers es de guapos: los 10 pantalones chinos más cómodos, refinados y al mejor precio para causar sensación en 2026</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Cultura y ciencia</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-12-22T19:00:00+01:00</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Póntelos para ir al trabajo, para una cita o simplemente para hacer recados por la ciudad. Los chinos de Dockers están a precio de derribo y te serán útiles en cualquier momento de este otoño-invierno</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Carlos Domínguez
+El año termina, toca dejarse de tonterías y apostar por lo que realmente vale la pena. No sé tú, pero de cara a este 2026 yo me quedo con Dockers. Porque no se trata de comprar por comprar, sino de elegir lo mejor. Son cómodos de verdad, de los que puedes llevar todo el día sin acordarte de que los llevas puestos, tienen precios ajustados y encajan con cualquier plan que tengas en la cabeza, desde ir a trabajar hasta una cena con amigos. Cuando una prenda funciona en tantos contextos, sabes que estás invirtiendo bien... Y aún más si está rebajada.
+Para mí, remodelar el armario en Año Nuevo pasa por quitar lo que no uso normalmente y quedarme con básicos que lo hacen todo más fácil. Los pantalones de Dockers tienen justo eso: calidad-precio difícil de igualar, tejidos que aguantan el trote y cortes que no pasan de moda. Te los pones con zapatillas, con botas o con zapatos y siempre quedan bien, la verdad. Y esa sensación de abrir el armario y saber que cualquier elección va a funcionar es, sinceramente, uno de esos pequeños placeres que te llevan a empezar el año con buen pie. ¡No te lo pienses!
+Dockers Smart 360 Flex Chino Tapered
+Si hablamos de versatilidad pura, el Dockers Smart 360 Flex Chino Tapered te salvarán la vida en más de una ocasión. Tienen corte tapered (más estrecho hacia el tobillo), que queda bien tanto con sneakers como con zapatos más formales, y el tejido Smart 360 Flex se estira lo justo para moverte sin restricciones, ya sea caminando, sentado todo el día en la oficina o improvisando planes después del trabajo.
+Encajan con prácticamente cualquier look que tengas en mente, lo que los convierte en un básico todoterreno para cualquier armario. Con ellos puedes hacer ese propósito de renovar con sentido sin gastar de más: son cómodos, elegantes sin pasarse y tienen ese equilibrio calidad-precio por el que Dockers lleva años siendo referencia en chinos. Si quieres empezar 2026 con prendas que funcionan de verdad, este modelo es un clásico.
+Dockers Go Active Flex
+El tejido Go Active Flex de estos Dockers se estira con naturalidad y vuelve a su sitio sin perder forma, así que tienen una gran ventaja: puedes agacharte, subir escaleras o pasar horas sentado sin sentirte atado. El azul marino es un color que no falla con nada: va con camisetas sencillas, camisas, jerséis o incluso alguna chaqueta más formal, lo que los vuelve extremadamente versátiles.
+Para mí, estos pantalones son de los que terminas usando más de lo que pensabas: cómodos para todos los días, lo bastante pulidos para salir a cenar y lo bastante tranquilos para el plan más casual del finde. Si tu propósito para 2026 incluye armario más práctico y menos caos cada mañana, este modelo Go Active Flex es una pieza clave que cumple en todos los frentes posibles.
+Dockers Slim Tapered Fit Easy Khaki
+Con los Dockers Easy Khaki Slim Fit en beige me pasa algo curioso: son de esos pantalones que te pones “sin pensar” y, aun así, siempre funcionan. Me gusta porque el corte slim estiliza sin apretar y el color beige tiene ese punto luminoso que levanta cualquier look, incluso los más básicos. Los llevo igual con una camiseta blanca y zapatillas que con camisa y zapatos, y siempre tengo la sensación de ir bien vestido sin haberme complicado lo más mínimo.
+Por si fuera poco son comodísimos, y eso para mí ya es media batalla ganada. En un momento en el que intento comprar menos pero mejor, estos Easy Khaki encajan a la perfección: versátiles, atemporales y fáciles de combinar con todo lo que ya tengo en el armario. Vamos, un pantalón que no hace ruido y acaba siendo protagonista más veces de las que esperaba.
+Dockers Signature Khaki Slim Fit
+En cuanto a los Dockers Signature Khaki Slim Fit Pants en gris (magnet), tengo una relación de confianza absoluta: son chinos que nunca te fallan cuando quieres ir bien vestido. El gris es un color comodín (no roba protagonismo, pero eleva el conjunto) y el corte slim fit te da una línea moderna sin apretar, lo justo para sentirte cómodo sin parecer informal. Cuando los necesito para una reunión, una cena o un plan que puede torcerse entre casual y arreglado, siempre acaban siendo mi elección.
+Lo que más me flipa de este modelo es ese equilibrio entre comodidad y presencia: no son pantalones que se arruguen a la primera, se comportan bien todo el día y combinan con casi cualquier cosa que tengas en el armario. En mi propósito de construir un guardarropa que funcione sin pensar demasiado, estos chinos Signature Khaki hacen honor a su nombre: clásicos, fiables y listos para acompañarte adonde sea.
+Dockers Straight Fit Signature 2.0 Khaki
+Tengo la sensación de que los Dockers Straight Fit Signature 2.0 Khaki Pants en color beige (New British Khaki) significan volver a lo esencial con estilo moderno. El corte straight fit es perfecto si no quieres ir ni muy ajustado ni muy ancho: simplemente cae bien, se siente cómodo y respira con cada movimiento. Y ese tono New British Khaki tiene una vibra clásica que levanta cualquier outfit, algo que para mí es clave cuando no quiero pensar demasiado por las mañanas.
+Lo mejor de este modelo es que son creaseless de verdad: los sacas del armario, te los pones y mantienen la forma incluso después de un largo día de trabajo o de un plan improvisado después de cenar. No tengo que estar arreglándolos cada dos por tres, y eso para mí vale oro cuando quiero ropa que trabaje conmigo, no al revés. En mi misión de tener un armario práctico y elegante para 2026, estos chinos straight fit se han convertido en una de esas piezas que funcionan solas.
+Dockers Alpha Original Khaki
+Cuando me pongo los Dockers Alpha Original Khaki en azul (Pembroke Blue), siento que tengo un comodín extra en el armario: no es el típico beige que todo el mundo espera, pero tampoco es un color que choque con nada. Ese azul Pembroke Blue tiene un punto sofisticado sin pasarse, y eso hace que los chinos funcionen igual de bien con una sudadera relajada que con una camisa si la ocasión lo pide. Son de esos pantalones que te salvan el look sin que te enteres.
+Además, con el corte clásico de la línea Alpha Original, hay espacio para moverse con naturalidad sin perder un aspecto pulido, lo que los convierte en mi elección favorita cuando quiero sentirme cómodo pero con estilo definido. En mi plan de darle sentido al armario este 2026, estos chinos azules no solo aportan variedad, sino que también amplían mis opciones.
+Dockers Ultimate 360 Chino Slim
+Basta con ver estos Dockers y saber que tienen personalidad propia. Cuando te los pones, te das cuenta de que se adaptan a todo. Ese color Dark Ginger no es el típico beige o azul que ves en cada esquina, tiene un punto cálido y diferente que hace que cualquier combinación (desde una sudadera relajada hasta la camisa más formal) se vea bien. Y con el corte slim, la silueta queda definida sin apretar, justo lo que busco.
+Lo que más me mola es la sensación de elasticidad real: el tejido se mueve contigo, no contra ti, lo que resulta perfecto para días largos en los que vas de aquí para allá sin parar. Para mí, estos chinos te acompañan tanto en un plan casual como cuando necesitas ir un pelín más arreglado sin parecer disfrazado. Si este 2026 quiero un armario que funcione en cualquier escena, los Ultimate 360 en Dark Ginger merecen un hueco.
+Dockers Go Airweave Chino Slim
+El color Sahara Khaki de los Dockers Go Airweave Chino Slim tiene un tono tierra que funciona con casi todo (camisetas claras, jerseys oscuros o incluso camisas estampadas) y no sé, es como si animara cada conjunto casi sin querer. El corte slim te da una línea moderna sin apretar, así que te ves bien sin sentirte encorsetado, lo que a mí me viene de maravilla cuando quiero ir bien sin pensar demasiado.
+Si algo me mola realmente de estos Dockers es el tejido Airweave: se siente ligero, fresco y muy agradable sobre la piel, incluso cuando el día se alarga o sube un poco la temperatura. Son pantalones que puedes usar de lunes a domingo, ya sea para currar, salir con amigos o para escapadas improvisadas. En mi idea de tener un armario funcional para 2026, los Go Airweave en Sahara Khaki son de esos básicos que siempre caen bien: confortables de verdad y listos para cualquier plan.
+Dockers Alpha Original Skinny
+Los Dockers Alpha Original Skinny son la versión más pulida de un chino clásico, aunque con una silueta más actual y definida. No es el típico slim que te aprieta por todos lados; es un corte skinny bien trabajado que sigue tu forma sin parecer restrictivo, lo que los hace perfectos tanto para looks casuales como para ocasiones en las que quieres ir un poco más arreglado.
+Su diseño pega con prácticamente cualquier cosa que tenga: desde una camiseta básica y zapatillas hasta una camisa ligera y botas si hace un poco más de fresco. En mi lista de propósitos para 2026, uno de ellos es tener prendas que simplifiquen mis elecciones diarias, y estos chinos Alpha Original Skinny encajan como anillo al dedo: cómodos, con un corte actual y un look que no falla, sean cuales sean mis planes.
+Dockers Classic Fit Easy Khaki
+Acabamos con los Dockers Classic Fit Easy Khaki Pants, con los que tengo una relación de puro confort desde que los descubrí: te los pones y te olvidas de que los llevas, con un acabado que siempre queda bien. El corte clásico no te aprieta ni se te va de formas raras, simplemente cae natural y te deja moverte sin ninguna molestia, cosa que valoro un montón cuando tengo días largos o planes improvisados. Para mí, que busco comodidad y estilo, estos Easy Khaki son un comodín valioso.
+Y lo mejor es que encajan con cualquier rollo que me apetezca: desde camiseta y zapatillas para un paseo tranquilo hasta una camisa más formal si surge una cena de última hora. En mi propósito de tener un armario eficiente, cómodo y sin dramas en 2026, estos Classic Fit se han ganado un sitio fijo: porque van con todo, se sienten bien todo el día y, honestamente, hacen que vestirse sea mucho menos conflictivo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>El Mundo</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C49" s="5" t="inlineStr">
+        <is>
+          <t>Vicente Vallés: "El libro sobre este PSOE se titularía 'Caos'. Leire Díez, Koldo... Personajes que se supone vienen de la nada. Son situaciones ridículas y absurdas"</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Cultura y ciencia</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-12-23T00:11:46+01:00</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Es la estrella de los Informativos de Antena 3, con todo lo que eso conlleva. Ha publicado 'La caza del ejecutor', una novela sobre geopolítica con China y Rusia como protagonistas Leer</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Pregunta.- ¿Cuál es la pregunta más impertinente que le han hecho?
+Respuesta.- '¿De qué equipo eres?'. Es una impertinencia intolerable que alguien me pregunte eso. Solo la duda es inadmisible y me ofende".</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>El País</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C50" s="5" t="inlineStr">
+        <is>
+          <t>Golden Goose, las zapatillas desgastadas de 2.000 dólares cada par, son un raro triunfo para el capital riesgo</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-12-26T05:30:00+01:00</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>La peor recesión del lujo desde la pandemia ha sido beneficiosa para la marca italiana y ha favorecido el precio de su venta al fondo chino HSG</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>La peor recesión del lujo desde la pandemia ha sido beneficiosa para la marca italiana y ha favorecido el precio de su venta al fondo chino HSG
+Golden Goose es un fabricante italiano dezapatillas deportivas de aspecto sucio y desgastadoque pueden llegar a costar 2.000 dólares un par. El precio de más de 2.500 millones de euros (2.900 millones de dólares) que su accionista de capital privado acaba de conseguir por la empresa de moda es también un monto más extravagante que desaliñado.
+La venta de la marca por parte de Permira al fondo chino HSG, anteriormente conocida como Sequoia Capital China, con Temasek de Singapur como inversor minoritario, es una de las pocas salidas exitosas del capital riesgo. Antes, se han dado una serie de problemas en ciertos acuerdos de adquisición alcanzados por el capital riesgo mientras el mundo salía de la pandemia, justo antes de que se dispararan los tipos de interés.
+La transacción de Golden Goose, que duplicala compra de Versace por parte de Pradade principios de este año, también se produce en un momento de baja demanda de artículos de lujo. La valoración puede ser menos chocante de la que se planteó en su plan de oferta pública inicial, un proyecto abandonado hace 18 meses, pero la firma de capital riesgo prácticamente ha duplicado el valor de la compañía en cinco años.
+Permira adquirió en 2020 la mayor parte de Golden Goose a Carlyle por 1.300 millones de euros. El año pasado, el mercado se resistió a considerar un valor empresarial de 3.000 millones de euros en su salida a la bolsa en Milán, y el plan fracasó. Los inversores señalaban los problemas de Dr. Martens, otra empresa de calzado anteriormente propiedad de Permira. La desaceleración del mercado de productos de alta gama no ayudó tras tres años de crecimiento vertiginoso.
+Y, sin embargo, la peor recesión del lujo desde la crisis financiera (excluyendo la pandemia) ha sido beneficiosa para Golden Goose.
+Mientras los consumidores acomodados, pero no superricos, controlaban su gasto, megamarcas como Louis Vuitton y Gucci subieron de categoría para seguir el ritmo del dinero. Al concentrarse en el 1% más rico, algunas marcas abandonaron productos básicos como las zapatillas de diseño, dejando ese mercado en manos de Golden Goose. También subieron los precios de zapatos, bolsos y otros productos básicos. El coste medio de una cesta de artículos de lujo icónicos en Europa aumentó un 54% entre 2019 y finales de 2024, según analistas de HSBC Holdings.
+A modo de comparación, Golden Goose ha subido los precios tan solo un 4% en los últimos cinco años. Esto hace que sus zapatillas, con un precio medio de 550 euros, incluyendo la personalización, tengan una mejor relación calidad-precio.
+La compañía aumentó las ventas de 266 millones de euros en 2020 a 655 millones de euros en 2024. El crecimiento ha continuado este año, con un aumento del 13% en las ventas en los primeros nueve meses y un 7% en el beneficio. Asumiendo un crecimiento similar para todo el año y un margen de Ebitda estable, Golden Goose podría generar alrededor de 740 millones de euros en ventas en 2025 y cerca de 250 millones de euros de Ebitda.
+El precio pagado por HSG equivale a aproximadamente 10 veces el Ebitda, un descuento respecto a las 13 veces de otra marca como Moncler y las 11 veces de Birkenstock, pero aún así duplica al menos el valor patrimonial. Permira se mantendrá como inversor minoritario.
+HSG anteriormente respaldó al fabricante de Labubu, Pop Mart, al propietario de TikTok, ByteDance, y a la plataforma china de redes sociales Red Note, por lo que la expansión de Golden Goose probablemente se centrará en Asia. Las zapatillas italianas únicamente generan el 12% de sus ventas en la región, y solo el 7% en China, una cifra muy inferior a la de la mayoría de las marcas de lujo. Aproximadamente la mitad de sus ventas se concentran en América; el resto, en Europa y Oriente Medio.
+Claramente, hay más opciones en China. Dado que los bolsos de Gucci y los zapatos de salón de Chanel ya no son tan apreciados, existe un gran interés por artículos originales que conecten emocionalmente con los jóvenes compradores.
+Un ejemplo son los zuecos de Crocs, que se pueden personalizar y se han convertido en un éxito entre los consumidores de la Generación Z del país. Esto es un buen augurio para Golden Goose. Las zapatillas deportivas representan el 90% de las ventas de la compañía, por lo que hay margen para diversificarse. Los bolsos y la ropa, que también se pueden personalizar, son otras oportunidades tanto en EE UU como en China. La experiencia de Temasek como inversor en Stone Island, Ermenegildo Zegna y el holding del presidente de Moncler, Remo Ruffini, debería ser de ayuda. El exdirector de Gucci, Marco Bizzarri, asumirá la presidencia.
+Pero alcanzar el objetivo a largo plazo de Golden Goose de elevar las ventas anuales a 1.000 millones de euros no será fácil. Aunque se espera que el mercado de lujo chino haya pasado lo peor, cualquier recuperación llevará tiempo. Y los consumidores locales se centran más en las zapatillas deportivas que les ayudan a correr más rápido o afrontar rutas más exigentes. Nike declaró recientemente que se la consideraba más una marca de calzado de moda informal que de alto rendimiento, lo que frenó las ventas y la obligó a rebajar los precios.
+Mientras tanto, las grandes marcas de lujo han decidido recuperar a sus clientes de clase media. Las zapatillas deportivas y productos similares serán clave, generando mayor competencia. Si Golden Goose logra expandirse con éxito en China y convertirse en una marca de estilo de vida más amplia como Ralph Lauren, su futuro se aleja de lo desaliñado. Pero dadas las dificultades de los propietarios de capital riesgo en los últimos dos años, no es mal momento para retirar dinero.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>El País</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C51" s="5" t="inlineStr">
+        <is>
+          <t>El automóvil busca ‘democratizar’ el eléctrico con coches por debajo de 25.000 euros para competir con China</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Negativa</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2025-12-25T05:15:00+01:00</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Cerrado ya el frente con la UE por los objetivos de emisiones, el sector apunta en 2026 a una ofensiva de producto con la que extender la movilidad eléctrica en el Viejo Continente</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Cerrado ya el frente con la UE por los objetivos de emisiones, el sector apunta en 2026 a una ofensiva de producto con la que extender la movilidad eléctrica en el Viejo Continente
+El año que está a punto de acabar ha estado marcado por dos victorias de calado para los fabricantes de coches en el ámbito de la regulación europea.La primera, que tuvo lugar en marzo, fue la suspensión para 2025 y 2026 de las multas para aquellas marcas que incumplan los objetivos de emisiones de CO2 de los coches nuevos que establece la normativa CAFE, que entró en vigor en enero. Tras presionar a la Comisión Europea, esta estableció que las emisiones del periodo 2025-2027 se contarán de forma conjunta, por lo que las sanciones se posponen, dando más tiempo a los fabricantes para incrementar sus matriculaciones de eléctricos. La segunda, se produjo este diciembre, con el anuncio de la Comisión Europea deflexibilizar los objetivos de emisiones para 2035: ese año, finalmente no se prohibirá la venta de vehículos de combustión.
+Cerrados ya esos frentes, sobre todo gracias a la presión de los grandes fabricantes de automóviles alemanes, ahora el sector apunta a un 2026 en el que tendrá que saltar al campo de juego y disputar el partido con las marcas chinas. El sector necesita volver a aumentar ganancias traslos pronunciados descensos de este año—algo en lo que han influido, y mucho, los aranceles aprobados por la administración estadounidense de Donald Trump—. Para ello, el motor lanzará al mercado una batería de coches eléctricos deen torno o por debajo de la barrera de los 25.000 euros sin contabilizar ayudas. Y ahí, España jugará un papel importante: buena parte de estos modelos se harán en el país, concretamente en las plantas del grupo Volkswagen en Navarra y Barcelona. La primera ensamblará el Volkswagen ID. Cross y el Skoda Epiq; mientras que la segunda hará el Cupra Raval y el Volkswagen ID. Polo.
+Volkswagen ha asegurado en varias ocasiones que estos modelos sonsu apuesta para “democratizar” la movilidad eléctrica, aunque de cara a 2027 apuesta por lanzar un modelo por debajo de los 20.000 euros, que se hará en Portugal. La Península Ibérica será su centro de producción de vehículos eléctricos asequibles, algo indispensable si quiere cumplir con los objetivos de emisiones de los próximos años. Renault, por su parte, comenzará a entregar a principios de año las primeras unidades de sunuevo Twingo, un modelo eléctrico por debajo de los 20.000 euros sin ayudas.
+Estos modelos serán aún más baratos en España al sumarlas ayudas públicas a la compra del Plan Auto+en el que trabajan el Ministerio de Industria y la patronal de fabricantes de coches, Anfac, que servirá para subvencionar las compras que se hagan a partir del 1 de enero. Hasta entonces seguirá operando el Moves y la deducción de un máximo de 3.000 euros en el IRPF por la compra de un electrificado.
+Las nuevas ayudas, sin embargo, también servirán para subvencionar la compra de eléctricos de los competidores chinos, que han encontrado en España su punto de entrada preferido a Europa. Ganvam, patronal que representa a los concesionarios y a los talleres, destacóen su encuentro de prensa navideñoque las marcas chinas tienen el doble de penetración en España que en el resto de la UE, con una cuota de mercado del 10%.
+A las ya conocidas por el público español como BYD, MG u Omoda, se sumarán el año que viene otras como Great Wall Motor (GWM) —que en un principio había desistido del mercado europeo, pero en octubre anunció el lanzamiento de siete modelos para el Viejo Continente—, Changano Lepas. Esta última pertenece al grupo Chery, que ya cuenta en Europa con otras marcas como Jaecoo y Ebro. Ello supone más competencia para fabricantes como Volkswagen, Renault o el grupo Stellantis, que en el ámbito del coche eléctrico acaban de presenciar la llegada al mercado dela versión más barata del Tesla Model 3. Con él, la compañía de Musk busca recuperar algo del inmenso terreno perdido este año, en el queha cedido mucha cuota de mercado.
+El Kia EV2, el modelo eléctrico más asequible hasta la fecha de la marca surcorena, que se hará en Europa, asoma también como un fuerte contendiente para las firmas tradicionales. Su hermano mayorEV3 fue el segundo eléctrico más vendido en España entre enero y noviembre, solo por detrás del Tesla Model 3.
+Más allá de la batalla entre los fabricantes de coches, España buscará atraer más inversiones industriales para afianzar su posición como unhubeuropeo de electromovilidad. Para ello se ha lanzado el Plan España Auto 2030, en el que se contempla aumentar entre 300.000 y 400.000 unidades la producción anual de coches, lo que equivale a la actividad de una planta estándar. El plan irá acompañado, además de ayudas a la compra y a la instalación de puntos de recarga en carretera, deun nuevo Perte del Vehículo Eléctrico y Conectado (Perte VEC) dotado con 580 millones de euros.
+A ese programa es posible que apunten algunos fabricantes chinos que ven a España como candidata a albergar una nueva planta, como son los casos de GWM, BYD o MG. Otro fabricante al que se busca seducir es a Renault, compañía que cuenta con dos plantas en Palencia y Valladolid, que a día de hoy están orientadas exclusivamente a la producción de híbridos. La compañía está centrada en llenar sus fábricas francesas de eléctricos, donde tiene una capacidad máxima de producción de 600.000 al año, algo que parecemás encaminado tras el acuerdo firmado con Ford para hacer dos modelos de la estadounidense en Francia. El objetivo del grupo galo es hacer un millón de eléctricos anuales en 2031 y para ello necesitará producir en otros países como España. Si bien la automovilística aún no ha confirmado la fabricación de sus primeros eléctricos en el país, seráun tema que se tratará en la negociación del nuevo convenio colectivoque entrará en vigor en 2026.
+¿Quieres añadir otro usuario a tu suscripción?
+Si continúas leyendo en este dispositivo, no se podrá leer en el otro.
+¿Por qué estás viendo esto?
+Si quieres compartir tu cuenta, cambia tu suscripción a la modalidad Premium, así podrás añadir otro usuario. Cada uno accederá con su propia cuenta de email, lo que os permitirá personalizar vuestra experiencia en EL PAÍS.
+¿Tienes una suscripción de empresa? Accedeaquípara contratar más cuentas.
+En el caso de no saber quién está usando tu cuenta, te recomendamos cambiar tu contraseñaaquí.
+Si decides continuar compartiendo tu cuenta, este mensaje se mostrará en tu dispositivo y en el de la otra persona que está usando tu cuenta de forma indefinida, afectando a tu experiencia de lectura. Puedesconsultar aquí los términos y condiciones de la suscripción digital.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>El País</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C52" s="5" t="inlineStr">
+        <is>
+          <t>La telenovela navideña con capítulos más cortos que TikToks</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Cultura y ciencia</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2025-12-25T05:30:01+01:00</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Se estrena el primer microdrama nacional, un género con episodios de entre uno y tres minutos que ha arrasado en China y América</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Se estrena el primer microdrama nacional, un género con episodios de entre uno y tres minutos que ha arrasado en China y América
+Con la cremallera del plumas de estampado más veraniego imaginable hasta arriba y un suéter cuello cisne, baila frente al espejo del baño. La voz corpórea de un narrador nos la presenta: es Sofía, treintañera o casi; las navidades las va a pasar esquiando con su novio. Porque lo quiere —nos explica ese timbre cálido y resonante— y porque —asumimos nosotros— cualquier plan le apetece más que la regresión que supone cada vuelta a casa, con papá y mamá empeñados en infundirle el júbilo de las fiestas por la fuerza. Se cruzan unos mensajes, su hermano avisa en el grupo familiar de que llevará a su nueva novia, “¡qué bien, al fin la conoceremos”. Va a librarse, sí, hay alivio en su rostro reflejado en el cristal. Hasta que encuentra unpost-itque lo trastoca todo: ni Baqueira ni novio. Fin del capítulo. Un minuto escaso de metraje.
+Ya han llegado a España.Una novia por navidad,recién estrenada,es la primera producción nacional de este género;microdramas, los llaman. Series rodadas en formato vertical en las que cada episodio no dura más de un par de minutos, ficciones pensadas para consumirse como vídeos de TikTok o Reels de Instagram, el algoritmo haciendo equipo con el viejo poder de la narrativa de giros de guion ycliffhangers(odio los anglicismos, pero qué visual es este) para tenernos a todos así: abismados frente a la pantalla del móvil.
+Un reportaje de El País Semanalde comienzos de año ya daba muestras del músculo en China de esta industria tan bisoña: sus ingresos en 2024, unos 6.685 millones de euros, habían superado a la taquilla de cine, según la Asociación de Servicios de Difusión por Red de China. Casi 600 millones de espectadores. A lo largo de este 2025, las microseries fueron conquistando fronteras nuevas, India, Estados Unidos y Latinoamérica, sobre todo, tierras fértiles en materia folletinesca.
+Ahora, me consta, también en Europa las productoras se han sumado a la fiebre de perseguir y cazar antes que la competencia a quien sea capaz de escribir y rodar estos argumentos tan esquemáticos como adictivos. Espadachín solitario salva el mundo, chica conoce a un buen mozo que no es lo que parece, romance erótico, repleto de frases para ligar que jamás pronunciaría alguien sensato en una discoteca; vampiros que parecen (y tal vez sean) la enésima reencarnación de Edward Cullen. Atresmedia, en su ficción de 60 capítulos, ha apostado por otra trama clásica: un triángulo amoroso, con parientes afectados.
+Sofía, a la que da vida la violinista y actriz Marina Baeza, con el mismo abrigo y botas rojas bajo un sol radiante, está sentada en un talud, junto a un camino. Comiendo polvorones. “¿Sabes que cada año mueren 23 personas atragantadas con los polvorones? Lo leí en un artículo. En Vogue”. La corredora que se le acerca preocupada por su salud es la creadora de contenido Carla Flila (casi un millón de seguidores en su cuenta de Instagram, entre ellos famosas como Rosalía o Carolina Yuste). Sofía, borde primero con la desconocida, no tarda en derrumbarse y en confesarle su desgracia: ¿qué clase de novio te abandona con una mera frase manuscrita en un papelito adherido a un azulejo antes de navidad? Entre las dos surge algo, complicidad, quizá un atisbo de atracción. Pero, por si la sugerencia no resultara meridiana, vuelve a actuar el narrador, que nos explica otro (maldito) anglicismo: “Acaba de suceder unmeet cute,expresión anglosajona que se refiere a la escena en la que dos personas que formarán una futura pareja romántica se encuentran por primera vez”.
+¿Y dónde descubre Sofía que el personaje que interpreta Flila es la novia de su hermano? En la ducha, por supuesto.
+Son tiempos de atención dividida, de vida a doble pantalla. La parte buena es que, si como yo aborrecen la navidad, en lo que tardan en escabullirse entre el gentío de las calles del centro, en lo que escapan de los cuartetos de cuerda callejeros que tocan el canon de Pachelbel, pueden haberse tragado 10 o 12 capítulos de las andanzas de Sofía. Hay navidades peores que las nuestras.
+¿Quieres añadir otro usuario a tu suscripción?
+Si continúas leyendo en este dispositivo, no se podrá leer en el otro.
+¿Por qué estás viendo esto?
+Si quieres compartir tu cuenta, cambia tu suscripción a la modalidad Premium, así podrás añadir otro usuario. Cada uno accederá con su propia cuenta de email, lo que os permitirá personalizar vuestra experiencia en EL PAÍS.
+¿Tienes una suscripción de empresa? Accedeaquípara contratar más cuentas.
+En el caso de no saber quién está usando tu cuenta, te recomendamos cambiar tu contraseñaaquí.
+Si decides continuar compartiendo tu cuenta, este mensaje se mostrará en tu dispositivo y en el de la otra persona que está usando tu cuenta de forma indefinida, afectando a tu experiencia de lectura. Puedesconsultar aquí los términos y condiciones de la suscripción digital.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>El Mundo</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>Taiwán aprueba una ley que busca equilibrar el desarrollo de la IA con el bienestar social</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Tecnología industrial</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2025-12-24T02:52:52+01:00</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>El texto legislativo estipula que la implementación de la IA debe adherirse a siete principios fundamentales: sostenibilidad y bienestar, autonomía humana, privacidad y gobernanza de datos, ciberseguridad y protección, transparencia, equidad y no discriminación, y responsabilidad Leer</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>El Yuan Legislativo (Parlamento) de Taiwán aprobó este martes la Ley Básica de Inteligencia Artificial (IA), una normativa que insta al Ejecutivo a promover la investigación y el desarrollo de aplicaciones de IA al tiempo que prioriza el bienestar social, la equidad digital, la innovación y la competitividad.
+Según la agencia de noticias CNA, el texto legislativo estipula que la implementación de la IA debe adherirse asiete principios fundamentales: sostenibilidad y bienestar, autonomía humana, privacidad y gobernanza de datos,ciberseguridad y protección, transparencia, equidad y no discriminación, y responsabilidad.
+La Ley Básica, adoptada con el apoyo de los dos principales partidos de la oposición, el Kuomintang (KMT) y el Partido Popular de Taiwán (PPT), que cuentan con mayoría parlamentaria, también designa al Consejo Nacional de Ciencia y Tecnología (NSTC) como la autoridad rectora en materia de IA.
+El gobernante Partido Democrático Progresista (PDP), por su parte,expresó sus objeciones respecto al texto, puesto que las leyes básicas tradicionalmente no especifican una autoridad competente.
+La normativa contempla la creación, por parte del Yuan Legislativo, de un comité nacional de estrategia de IA, encabezado por el primer ministro e integrado por académicos, representantes de la industria, jefes de agencias gubernamentales y autoridades locales, con el mandato de formular directrices para el desarrollo de esta tecnología y reunirse al menos una vez al año.
+Asimismo,la nueva ley exhorta al Ejecutivo a asignar fondos para la investigación en torno a la IAy a proporcionar asistencia y subsidios para el desarrollo, la capacitación, las pruebas y la validación de la IA, según CNA.
+Hogar del principal fabricante de semiconductores (TSMC) y del mayor ensamblador de productos electrónicos del mundo (Foxconn), Taiwán se ha visto fuertemente beneficiado por el auge de la IA y de la computación de alto rendimiento: el PIB local anotó un avance del 8,21 % en el tercer trimestre de este año gracias al tirón de las exportaciones.
+El Gobiernoprevé que la fotónica de silicio, la computación cuántica y la robótica generen cientos de miles de empleosy billones de dólares taiwaneses en producción en las próximas décadas, mientras aspira a situar a la isla entre los cinco principales desarrolladores de inteligencia artificial en el mundo.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>El Mundo</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C54" s="5" t="inlineStr">
+        <is>
+          <t>El plan de Maduro para hacer frente a la Casa Blanca: ofensiva internacional, resistencia y desgaste de Trump, con apoyo de Rusia y China, sus aliados</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Geopolítica</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2025-12-23T19:30:19+01:00</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>El Consejo de Seguridad de la ONU celebra este martes una reunión extraordinaria a petición de Caracas para abordar la crisis en el Caribe Leer</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Es una carta de seis páginas, firmada porNicolás Maduro, pero que pareciera un publirreportaje pagado de la Venezuela que no existe. "Hoynuestra nación vive en paz, con estabilidad institucional, crecimiento económico sostenido y una firme vocación de diálogo y entendimiento entre los pueblos, pese a haber sido sometida durante años a medidas coercitivas unilaterales y presiones externas", asegura el "presidente pueblo" en la misiva dirigida a los mandatarios de América Latina y del Caribe, en la que mezcla sufalso victimismocon las claves principales de suestrategia internacional para atornillarse en el poderpese aldespliegue naval estadounidensey jaque petrolero diseñado por Washington.
+Como parte de la misma ofensiva contra la "piratería internacional" de EEUU se llevó a cabo ayerun consejo extraordinario, a petición de Maduro, del Consejo de Seguridad de Naciones Unidas, precedido del paso adelante de los tres grandes aliados globales del chavismo:Rusia, Irán y China. Serguéi Riabkov, viceministro ruso de Exteriores, insistió ayer que su gobierno ha mostrado a Washington supreocupación ante la escalada del conflicto, tras negar que estén evacuando a su personal diplomático de Caracas.
+"El mundo debe saber que la amenaza no es Venezuela, es EEUU. Venezuela sólo es el primer objetivo de un plan mayor para dividir y dominar a América Latina", predicó el embajador chavista, Samuel Moncada, en el Consejo de Seguridad. Rusia aprovechó el debate y respaldó a Caracas, su gran aliado en las Américas.
+EEUU, en cambio, no se achantó y aprovechó para adelantar que llegarán más sanciones y más fuertes"para privar a Maduro de los recursos que utiliza para financiar el Cártel (narco) de los Soles", precisó el embajador Mike Waltz, quien además aseguró que los petroleros de la flota fantasma que EEUU persigue en el Caribe "son el principal salvavidas de Maduro y su régimen totalitario".
+Varios de los participantes en esta reunión extraordinaria atacaron duramente a Caracas, como Argentina, que volvió a mostrar su apoyo ala máxima presión para sacar el ilegítimo Maduro del poder. Varios países europeos, como Francia, Reino Unido, Eslovenia y Dinamarca, criticaron las violaciones chavistas de los derechos humanos y reclamaron una vía de diálogo para salir del conflicto.
+No sólo Rusia, también China e Irán han irrumpido con fuerza en la crisis del Caribe tras la incautación de dos petroleros, uno con destino a Cuba y otro al propio país asiático.China es el principal cliente del petróleo venezolano, aunque parte de los pagos se realizan para condonar la deuda entre los dos países, que se acercaba a los 60.000 millones de dólares.
+"EEUU viola flagrantemente el Derecho Internacional en el Caribe, con el aumento de presión contra un gobierno independiente, con el objetivo de intervenir y cambiar la soberanía de ese país.La República Islámica responderá de manera adecuada ante cualquier agresióno ataque contra sus intereses", advirtió Esmail Baghai, portavoz del Ministerio de Asuntos Exteriores de Irán.
+De esta forma,Maduro ha regresado a la ONU cuando hace semanas se quejó de que no servía para nada. Además, en 2024, a raíz del encarcelamiento de la hispanovenezolana Rocío San Miguel, figura emblemática de la sociedad civil venezolana, el chavismo expulsó a la oficina de Derechos Humanos de Naciones Unidas, a la que más tarde permitió volver y a la que más tarde amenazó de nuevo.
+La ong Transparencia Venezuela, uno de los bastiones en la investigación de la corrupción revolucionaria, identificó en las últimas horas a 10 buques que están cargando o esperando cargar en puertos venezolanos."El negocio del petróleo es tan atractivo económicamente que mucha gente está dispuesta a correr riesgos", afirmó Mercedes de Freitas, al frente de Transparencia Venezuela.
+"Otra cosa que identificamos es que esos barcos entran y salen con petróleo y algunos van a China. Nosotros hacemos seguimiento a la aduana de China y no aparece que hayan recibido petróleo venezolano", desveló Freitas.
+En cambio, quien no ha dejado de fletar sus barcos entre Venezuela y EEUU es la multinacional Chevron, que según Reuters ha exportado siete cargamentos de petróleo, cada uno con entre 300.000 y 500.000 barriles, en lo que va de mes.El último buque cisterna, enviado el pasado domingo con destino al Golfo de México,contó con la supervisión de la vicepresidenta Delcy Rodríguez. Chevron puede operar en el país criollo gracias a las licencias concedidas primero por Joe Biden y después por el propio Trump.
+"La estrategia internacional de Maduro es resistir porque está consciente de las limitaciones que enfrenta. Con el bloqueo y confiscación de buques petroleros,vuelven a escena países como China y en menor medida Rusia porque sí tienen las herramientas para ayudar a Maduroa sortear el bloqueo selectivo, por ejemplo facilitando tanqueros que no estén sancionados o que tengan bandera de algún país como China que suba los costos para que EEUU confisque el barco. Creo que ahora mismo el régimen de Maduro trata justamente de convencer a países como China y Rusia que le otorguen esa ayuda, donde el riesgo de un enfrentamiento militar con EEUU es menor. En las próximas semanas quedará claro si hubo esa voluntad de tenderle una mano a Maduro, dada las estrechas alianzas que han formalizado con esos países", profundiza el internacionalista Mariano de Alba para EL MUNDO.
+Resistencia y jugar al desgaste de la administración Trump II, pese a la última andanada llegada desde Washington.El mandatario estadounidense empleó nuevas palabras ("Si se pone rudo, será la última vez que lo haga"), para mantener la presión contra el dictador bolivariano, a quien señalan como cabecilla del narco Cártel de los Soles.
+La respuesta se la dio ayer Diosdado Cabello, número dos de la revolución y ministro de Interior, rodeado de policías y militares en un acto mañanero de prietas las filas: "El Imperio (EEUU), más temprano que tarde, va a desaparecer por el bien de la Humanidad".
+Previamente, Maduro había aconsejado a Trump que se dedicara a los temas económicos y sociales en su país."Le iría mejor con el mundo si él atendiera los temas de su país. Cada presidente en lo suyo. Imagínate que yo perdiera mi tiempo metiéndome con otros países. Lo estaría haciendo muy mal", planteó el mandamás bolivariano, que cierra el año con la mayor inflación del planeta, triturada hace días la barrera del 500% de subida de los precios.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>Una misa del gallo global en 1592</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Cultura y ciencia</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2025-12-25T20:11:51+01:00</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Amediados de 1590, don García de Mendoza, marqués de Cañete y octavo virrey del Perú, despachó un navío a la China saltándose las prohibiciones reales, so pretexto de recaudar impuestos con los gravámenes que pensaba aplicar a las mercaderías orientales. Sin embargo, de los 300 mil ducados de plata embarcados en aquella nave, 100 mil habían salido del bolsillo del mismo virrey, lo que nos insta a poner en duda su repentino entusiasmo fiscal. Con todo, el barco fue interceptado por las autoridades portuguesas y aquellos duros antiguos que tanto en Macao dieron que hablar, nunca volvieron a manos ni del virrey ni de los mercaderes limeños que instigaron aquella operación de contrabando. ¿Quién se quedó con esos 300 mil... Ver Más</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>comentarios reales
+Fernando Iwasaki
+Esta funcionalidad es sólo para registrados
+Esta funcionalidad es sólo para registrados
+Amediados de 1590, don García de Mendoza, marqués de Cañete y octavo virrey del Perú, despachó un navío a la China saltándose las prohibiciones reales, so pretexto de recaudar impuestos con los gravámenes que pensaba aplicar a las mercaderías orientales. Sin embargo, de los 300...mil ducados de plata embarcados en aquella nave, 100 mil habían salido del bolsillo del mismo virrey, lo que nos insta a poner en duda su repentino entusiasmo fiscal. Con todo, el barco fue interceptado por las autoridades portuguesas y aquellos duros antiguos que tanto en Macao dieron que hablar, nunca volvieron a manos ni del virrey ni de los mercaderes limeños que instigaron aquella operación de contrabando. ¿Quién se quedó con esos 300 mil ducados, equivalentes a 20 millones de nuestros euros actuales?
+Al fallido negocio chino del marqués de Cañete dediqué uno de los capítulos de mi vieja tesis de maestría, donde descubrí que el testaferro del virrey y sus cómplices fue un jesuita sevillano: el padre Leandro Felipe, admirado por «haberlo sacado Dios del tumulto de los negocios». El marqués no dudo en meter de nuevo a Leandro Felipe en aquel berenjenal, porque nadie podía cuidar mejor la pasta gansa del señor virrey, que un jesuita versado en negocios. No obstante, quizá Dios no sacó del todo al sevillano del tumulto de los negocios, porque cuando Leandro Felipe comprendió que la Hacienda portuguesa se disponía a trincar los 300 mil ducados, del tirón los depositó en la caja jesuita de Nagasaki para socorrer las misiones de la Compañía de Jesús en el Japón. Si el dinero hubiera llegado a Portugal, sin duda el marqués de Cañete habría recuperado una parte, pero de la hucha de las misiones ya no lo sacaba ni Dios.
+El padre Leandro Felipe regresó a Lima diez años más tarde, porque su aventura nunca dejó de ser un episodio delictivo que supuso arrestos domiciliarios por colegios y conventos de Macao, Yemen, Goa, Malaca y México. Así, según la 'Monumenta Indica', Leandro Felipe pasó la Navidad de 1592 en el colegio de Goa (India), donde participó en una misa del gallo multicultural, pues «uvo sermón en diversas lenguas, scilicet, latín, ytaliano, portugués, castellano, inglés, vizcaíno, flamenco, francés, malavar, china, japón, griego, hebreo, canarín, del Pyrú y otras tres o quatro». Doctrinero en los Andes, el sevillano Leandro Felipe se arrancó a predicar en quechua en una misa del gallo celebrada en la India, cuando expiraba el siglo XVI.
+Ahora que ponderamos el legado civilizador de España durante la primera globalización, reparemos en cómo toda aquella diversidad se integró a través de una fiesta como la Navidad. Oro, incienso, mirra y un puñaíto de lenguas. Feliz Pascua de Navidad.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>La Vanguardia</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C56" s="5" t="inlineStr">
+        <is>
+          <t>“El gran ganador de este año es China”</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Geopolítica</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2025-12-26T06:00:00+01:00</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Plàcid García-Planas dibuja un mundo volátil con Oriente Próximo estancado, Europa “zombi” ante el abandono de Trump y Pekín llenando los vacíos, en un año donde la IA ya está en “vuestra nevera” y predice proteínas para curar enfermedades</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Departamento Audiovisual
+Barcelona
+“Tenemos paz estable, no. Lo que tenemos es una guerra estable”, resume Plàcid García-Planas, periodista de Internacional de La Vanguardia, sobre el conflicto en Gaza, donde “el sufrimiento continúa” con entre 16.000 y 18.000 heridos esperando tratamiento exterior. Lo que definirá el futuro, advierte, “no es tanto la derrota militar de Hamás o de los palestinos, sino el abandono que todos los países árabes han tenido de la causa palestina”, ya que ningún gobierno rompió con Israel pese a las críticas.
+Para 2026, “lo único seguro es que los palestinos continuarán sufriendo”, pronostica García-Planas, que rechaza análisis en “un mundo tan volátil” pero destaca el “pulso interno” en Israel entre “los duros, Netanyahu y los duros” y un “Israel liberal que aunque parezca que no exista, existe”. Sobre el plan de paz de Donald Trump, es pesimista: “¿Qué es plan y qué es paz para Trump? Para él, paz es negocio, para él, paz es el Nobel”, lo que hace “muy difícil” un acuerdo generoso con los palestinos.
+Ucrania redefine una Europa “zombi”
+La invasión rusa de Ucrania está en “una situación como de empate”, donde “ninguno es capaz de acabar de imponerse”, pero “acabará definiendo Europa”, insiste García-Planas. Europa vive “en plan zombi, todavía no sabe cómo salir” ante la “irrupción de Trump, que ha cambiado no solo la política. Los cambios son tan profundos que todavía no somos conscientes. Esto los libros de historia hablarán de este año como de un año esencial”.
+Estados Unidos “abandona Europa, la deja aparte” en su nueva estrategia de seguridad, “insulta Europa” y obliga al continente a “espabilarse” tras décadas de depender de su protección, lo que tendrá “consecuencias en todos los niveles”.
+En Latinoamérica, el giro a la derecha refleja que “la democracia funciona” y un “hartazgo de los gobernantes que habían llevado el país hasta ahora”, aunque Trump revive la doctrina Monroe con interferencias directas, como amenazas a Venezuela que nadie sabe si cumplirá.
+China, el gran ganador de la volatilidad
+“Lo que definirá el futuro es la volatilidad. Y el gran ganador de momento es China, porque China llena todos los huecos que abandona Estados Unidos”, sentencia García-Planas sobre un 2025 marcado por tuits imprevisibles de Trump que “lo tambalean todo”. El mundo avanza hacia “menos democracia” y “sistemas totalitarios”, con negociaciones agarradas “con pinzas” por la inestabilidad.
+IA predictiva revoluciona la ciencia
+Francesc Bracero, periodista de tecnología de La Vanguardia, distingue la IA predictiva, que predice “la estructura de proteínas” para elaborar medicamentos contra enfermedades incurables, de la generativa como ChatGPT. “La tenéis en vuestros televisores, en vuestra nevera... y ahora mismo está en la aspiradora”, asegura, destacando su rol en rutas de tráfico o chatbots administrativos como el nuevo de la Generalitat.
+La IA no ha restado tantos empleos como se temía –un 12% según el MIT–, porque “una máquina no puede empatizar” ni mantener contactos humanos innatos tras millones de años de evolución. Sobre la inteligencia artificial general, los expertos divergen: algunos ven agotados los grandes modelos de lenguaje y apuestan por enfoques nuevos que superen la humana en cálculo, mientras su impacto en industria y salud mental apenas empieza a vislumbrarse.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>La Vanguardia</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C57" s="5" t="inlineStr">
+        <is>
+          <t>Una “Flota Dorada” para Trump</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Geopolítica</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Amenaza</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2025-12-24T06:00:00+01:00</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>El presidente estadounidense promete ampliar la fuerza naval de su país en plena carrera con China</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Daniel R. Caruncho
+Barcelona
+En el mundo de Donald Trump, todo es dorado.
+Desde la decoración de la Casa Blanca –molduras áureas en cada rincón– a su nuevo visado para extranjeros multimillonarios –la llamadaGold Card–, pasando por el ambicioso proyecto de escudo antimisiles destinado a proteger a EE.UU. de ataques aéreos –la ya célebre Cúpula Dorada–.
+Oro por tierra, aire y también por mar: el magnate hace tiempo que fantasea con construir una “Flota Dorada” para insuflar una nueva vida a la Armada estadounidense, y el lunes dio un primer paso para materializar su sueño.
+En un acto ante la prensa en su residencia privada en Mar-a-Lago, Trump anunció el lanzamiento de una nueva clase de barcos de guerra –“acorazados”, según él, aunque en realidad se trata más bien de destructores– que llevarán su nombre.
+Estos buques, dijo el presidente estadounidense, serán “los mejores del mundo”, “cien veces más potentes” que cualquiera de los que se hayan construido hasta ahora. “Inspirarán miedo en nuestros enemigos”, aseguró el mandatario en su habitual tono grandilocuente.
+Imagen de uno de los buques “clase Trump”
+De acuerdo con las explicaciones de Trump, las nuevas embarcaciones pesarán entre 30.000 y 40.000 toneladas y estarán equipadas con la última tecnología, como inteligencia artificial y láseres de alta potencia. Además, podrán transportar misiles de crucero nucleares, un tipo de armamento del que los buques estadounidenses prescindieron al finalizar la guerra fría, cuando ya no era necesario marcar terreno ante la amenaza soviética.
+El magnate –que compareció junto a sus secretarios de Estado, de Defensa y de la Armada, en un atril flanqueado por plafones que mostraban recreaciones virtuales de los barcos decoradas con su efigie– aseguró que el programa comenzaría “casi de inmediato” con la construcción de dos buques, y que la idea era llegar a las 25 embarcaciones de este tipo.
+Para Trump, esta renovación de la flota militar es un asunto de máxima prioridad. “Necesitamos barcos con urgencia”, dijo. “Algunos de nuestros barcos se han quedado viejos y obsoletos, y vamos a ir en la dirección opuesta”, agregó el mandatario, que espera que su nuevo proyecto sirva para reanimar la industria naval de su país, creando “miles” de puestos de trabajo.
+De hecho, hoy EE.UU. va a la zaga de China en lo que respecta a poderío marítimo. Según datos del Departamento de Defensa estadounidense, el gigante asiático disponía en el 2023 de 332 embarcaciones de guerra, frente a las 291 de la superpotencia norteamericana.
+Los astilleros chinos echan humo: de ahí han salido cerca del 60% de las embarcaciones construidas en todo el mundo este año (incluyendo las de uso civil). Y no parece que vayan a aflojar el ritmo. Pekín está regando de dinero el sector, consciente de que el futuro de la hegemonía globalpasa por el control de los océanos.
+Eso sí, este predominio tiene sus sombras: los buques y submarinos chinos no han sido testeados en situación de combate, a diferencia de los estadounidenses, por lo que su fiabilidad está en duda.
+Pero esto es un consuelo menor para EE.UU., que se ve incapaz de igualar la hiperproducción de su rival.
+El Centro de Estudios Estratégicos e Internacionales, con sede en Washington, alertaba en un informe reciente de que la industria naval estadounidense arrastra serios problemas que le impiden cumplir con las demandas de modernización de la flota de guerra: falta mano de obra especializada, las infraestructuras no están a la altura y la cadena de suministro es muy frágil.
+Estos obstáculos, imposibles de eliminar de un día para otro, pueden echar por tierra las aspiraciones de Trump, que en los últimos meses ha visto cómo la Armada tenía que cancelar iniciativas como el programa de fragatas Constellation, que acumulaba tres años de retraso y que debía producir buques bastante más sencillos que los de la “Flota Dorada”.
+El presidente estadounidense dijo el lunes que esperaba tener listo su primer barco en dos años y medio, pero ese calendario parece poco realista. No solo no existe todavía un diseño detallado de los buques, sino que todos los astilleros están saturados, por lo que es difícil que puedan hacer hueco a un encargo de estas características. Los precedentes más inmediatos tampoco invitan al optimismo: la última vez que EE.UU. se propuso crear un nuevo tipo de barco de guerra –eldestructor Zumwalt– se necesitaron cinco años para completar el proceso, que además terminó en fiasco, con sobrecostes multimillonarios.
+Y más allá de que el proyecto de Trump sea poco viable, están las dudas sobre su idoneidad. Numerosos analistas militares consideran que el armamento de los nuevos buques de guerra es poco práctico, y que no se adapta a las necesidades reales de la Armada.
+El contralmirante retirado Mark Montgomery era tajante ayer en la cadena ABC: si EE.UU. construye los buques de la “clase Trump” cometerá un gran error. Son barcos demasiado grandes y caros (cada uno puedo llegar a costar unos 10.000 millones de dólares), y poco adecuados para enfrentarse a China.
+Pero esas críticas no parecen hacer mella en el ánimo de Trump, el presidente cegado por el color dorado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>La Vanguardia</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C58" s="5" t="inlineStr">
+        <is>
+          <t>China se proyecta como potencia en la Antártida</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Geopolítica</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>2025-12-23T17:00:59+01:00</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Una nueva “ley de asuntos antárticos” regula aspectos “turísticos, navieros y pesqueros” en el continente</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Jordi Joan Baños
+Bangkok. Corresponsal
+Puesta a elegir entre la Luna y la Antártida, China ha decidido que se queda con las dos. Esta semana ha presentado un proyecto de ley que codifica su creciente presencia en el continente helado, con vistas a jugar un papel mayor en su gobernanza.
+La denominada “ley de asuntos antárticos” busca proteger sus intereses como estado, pero también regular las actividades de sus propios ciudadanos, en armonía con el medio ambiente. Los chinos son la segunda nacionalidad entre los turistas que, en grupos organizados, se acercan a la Antártida durante el verano austral, a partir de Punta Arenas (Chile) o Ushuaia (Argentina).
+Es cierto que los estadounidenses todavía son cuatro veces más.  Pero con la puesta en funcionamiento de la tercera base permanente en la Antártida, hace un año, China ha alcanzado la paridad con otros potencias antárticas, como EE.UU.. Siguen por delante Rusia y las dos república del  Cono Sur. China cuenta además con dos bases temporales (España tiene una), lo que eleva el total a cinco.
+Cabe recordar que la Antártida es territorio desmilitarizado y no sujeto a explotación económica. Junto a los pingüinos, solo viven allí comunidades de científicos (un millar en invierno y cinco veces más en verano). No está en el centro del huracán geopolítico, como  el Ártico, pero está dejando de estar en el limbo.
+El comité permanente del Congreso Nacional del Pueblo revisa desde el lunes el proyecto de ley antártica. Un movimiento coherente con la intención de China de jugar un papel más relevante en ambos polos, aunque no se cuente entre los países del Consejo Ártico. China se describe como “país casi ártico”, pero lo cierto es que es un mero observador, como España.
+Una de las bases chinas en la Antártida, donde Pekín cuenta con tres estaciones permanentes y dos temporales.
+La diferencia es que China es también la gran fábrica del mundo y potencia exportadora, por lo que observa con interés las rutas árticas -antaño heladas casi todo el año- que se van despejando con el aumento de las temperaturas. Habla ya de las Rutas Polares de la Seda, que le permitirían durante parte del año recortar en más de un 50% la singladura hasta el Atlántico Norte, en comparación con la ruta del canal de Suez. Evitando, además, el estrecho de Malaca.
+La China de Xi Jinping pide más voz, de acuerdo con su actual peso económico. Una vez más, podría chocar con EE.UU., cuyo presidente Donald Trump pretende todo lo contrario: impugnar el orden comercial, manteniendo el status quo político.
+Está por ver cuál es el propósito último de China en la Antártida. El precinto que la rodea podría no ser eterno. Su actual condición de paraíso natural limita la utilidad de sus 18.000 kilómetros de costa. Aunque la ruta austral recortaría de forma modesta el trayecto entre Shanghái y Buenos Aires, todavía acarrea más riesgos que beneficios.
+En cualquier caso, la legislación antártica en estudio -para ciudadanos chinos o embarcados en expediciones chinas- ya no presupone que solo científicos con las espaldas cubiertas se desplacen allí. En 57 artículos, trata de turismo, pesca o navegación, con exigencia de itinerarios detallados, seguros y planes de impacto ambiental, con previsión de multas en caso de incumplimiento, así como vetos de uno a tres años.
+Rompehielos de investigación polar Xuelong y Xuelong 2 en la 42 expedición antártica china, el pasado día 5
+Tan Xianchun, investigador  de la Academia de Ciencias, dijo que, tras más de cuarenta años en la Antártida, China ha pasado del estadio de acumular capacidades al de definir las reglas, primando “el uso pacífico, la protección ambiental, la conservación de recursos, la cooperación internacional o el apoyo científico”.
+La legislación china observa por tanto la prohibición de actividades militares o la extracción de recursos minerales, “excepto para fines científicos”. Esta “exploración verde” propuesta para la Antártida tiene poco que ver, en fondo y forma, con los planes de Donald Trump para Groenlandia, pero eso no elimina las suspicacias.
+Por ejemplo, un documento presentado este mismo mes, por encargo del presidente de Francia, reconoce que la Antártida está en las antípodas del Ártico en todos los sentidos, pero alerta que “podría convertirse en el decenio que viene en el próximo objetivo estratégico de las tres grandes potencias”. “Estados Unidos, China y Rusia”, señala, “mantienen un tercio de las bases científicas permanentes en la Antártida y parecen proyectarse hacia una revisión del Protocolo de Madrid en lo relativo a la protección del medio ambiente antártico, cuando eso sea posible en 2048”.
+“Para entonces la explotación de los considerables recursos del Continente Blanco se impondrá a su protección”, concluye el enviado especial de Emmanuel Macron para los Polos y el Océano, Olivier Poivre d'Arvor, que recomienda que la protección del Tratado Antártico no prescriba.
+Mientras China señala al Polo Sur, tiene un ojo puesto en la Luna, donde quiere enviar una misión tripulada a partir de 2030. Tras haberse convertido en el primer país en alunizar una nave no tripulada en la cara oculta -trayendo de regreso a la Tierra muestras del terreno- su próximo objetivo es encontrar hielo en el polo sur del satélite terrestre. También ensaya con impresoras 3D capaces de convertir el suelo de la Luna en ladrillos. En consonancia con su objetivo de establecer una base lunar permanentemente habitada, la década que viene, en colaboración con Rusia. EE.UU. agiliza sus propios planes de retorno a la Luna. La competición entre potencias desborda el espacio y alcanza los polos, de la Tierra y la Luna.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>La Vanguardia</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>Mensajes virales difunden desinformación sobre “oro falso” de China para vender criptomonedas</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Negativa</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>2025-12-26T06:00:00+01:00</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Un supuesto lingote de oro falso se utiliza para generar alarma y captar inversores principiantes</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Verificat
+Que está proliferando la comercialización de oro falsificado proveniente de China.
+Que, sobre la base de informaciones publicadas y evidencias recogidas por la policía, no hay ningún indicio de que se esté produciendo una circulación masiva de oro falsificado.
+Múltiples cuentas de redes sociales y en varios idiomas han viralizado en las últimas semanas mensajes sobre la supuesta proliferación de oro falsificado proveniente de China. Estos mensajes lanzan advertencias sobre el riesgo de invertir en oro para, seguidamente, mostrar las supuestas bondades de las inversiones en criptomonedas obviando el riesgo, o directamente enlazar a plataformas de inversión en línea de alto riesgo.
+Todos los mensajes detectados por Verificat llevan un mismo vídeo que muestra, aparentemente, un lingote de oro de China. No obstante, desde Verificat no hemos encontrado ninguna información fidedigna reciente de medios de comunicación ni instituciones oficiales que adviertan de un riesgo reciente de oro falsificado masivo en el mercado. La Policía Nacional tampoco tiene ninguna evidencia que demuestre la circulación de oro falsificado a gran escala. La mayoría de los mensajes virales masivos van en una misma línea: divulgar los supuestos beneficios de invertir en criptomonedas y, en algunos casos, atraer clientes inexpertos a inversiones en línea de alto riesgo. ¡Te lo explicamos!
+Los mensajes se han hecho virales sobre todo en la red social X (antiguo Twitter). Todos, independientemente de la red en la que circulen, llevan adjunto el mismo vídeo, que muestra un lingote con la inscripción “中国黄金” (“Oro de China”, en chino) y un logo en la parte superior identificativo de laChina National Gold Group Corporation, la empresa estatal dedicada a la gestión del oro en China.
+Imagen del vídeo viral
+Haciendo una búsqueda inversa de imágenes, desde Verificat no hemos encontrado ninguna publicación con información fidedigna que advierta sobre el contenido de los mensajes virales.
+Las evidencias más antiguas son del pasado septiembre. Uno de los primeros espacios masivos en que ha circulado el vídeo, según las evidencias encontradas, es un canal de Telegram con más de 89.000 suscriptores y editado en chino, que difundió una publicación en X que por sí sola no se ha hecho viral. Este canal de Telegram publica contenido crítico sobre el funcionamiento de las instituciones chinas y se hace eco también de hechos de países cercanos, como las revueltasdel pasado septiembre en Nepal.
+Algunos de los mensajes indican que varias empresas “han ganado casi 3.000 millones de dólares vendiendo oro falsificado a compradores particulares internacionales”, una cifra que difícilmente habrían pasado por alto los medios de comunicación generalistas. Sin embargo, ni en agencias de noticias internacionales ni en medios de comunicación de referencia se ha encontrado ninguna noticia que haga referencia a un fraude masivo reciente de oro falsificado proveniente de China.
+Además, el departamento de prensa de la Policía Nacional, preguntado por Verificat, ha explicado que el cuerpo policial no tiene ningún indicio sobre una supuesta circulación masiva de oro falso.
+Desde hace años, son habituales las estafas en línea que intentan vender inversiones de alto riesgo, por ejemplo criptomonedas, como si fueran movimientos seguros. Se dirigen a personas inexpertas con promesas de grandes ganancias en poco tiempo, según advierte el Instituto Nacional de Ciberseguridad (Incibe). Por ejemplo,en Verificatya hemos encontrado anteriormente casos de vídeos hechos con inteligencia artificial que suplantan la identidad de personas conocidas para dar apariencia de veracidad a los contenidos fraudulentos y así dirigir a las víctimas a dudosas plataformas de inversiones.
+Sobre las criptomonedas, la Agencia de Ciberseguridad de Catalunyarecuerdaque su valor puede experimentar “variaciones significativas” y que, por lo tanto, es una “inversión de alto riesgo y se puede llegar a perder todo lo que se ha invertido”. Además, avisa de que “las facilidades de anonimato hacen que sea un objetivo para los delincuentes”.
+La entidad CaixaBank, enun artículoen su blog, recomienda que, si alguien compra oro asumiendo el riesgo inherente que tiene esta operación, lo haga en un lugar que sea de máxima confianza. Una referencia para asegurar el valor de la compra, dice el artículo, es la misma Fábrica Nacional de Moneda y Timbre, una entidad pública empresarial de España adscrita al Ministerio de Hacienda.
+Con todo, el oro falsificado es una realidad. En 2022, por ejemplo, la Policía Nacional detuvo a dos personas por un delito de estafa por, presuntamente, vender lingotes de oro falsos en Valencia y Alicante, según explicó la Agencia EFE enuna noticia. En ambos casos, las cantidades eran de pocos miles de euros. Este tipo de estafas afectan sobre todo a quien compra el oro falso, que puede perder el valor de su inversión, pero es una cantidad insignificante para modificar el precio del oro en el mercado global.
+Asimismo, en un reportaje de 2019, la agencia de noticiasReuters explicóque existe un tráfico de lingotes de oro falsificado desde China que acaba en el mercado global. La agencia detalla que los lingotes que usan metal barato recubierto en oro son “fáciles de detectar” y que el problema está en lingotes de oro de verdad que tienen sellos falsificados de refinerías de prestigio. Estos lingotes sirven para burlar medidas globales de bloqueo de minerales de conflictos o de prevención de blanqueo de capitales.
+El medio financiero estadounidense CNBC tambiéninformó el año pasadosobre el problema del oro falsificado en China que, según añade, afecta a compradores de oro chinos dentro del país.
+Verificat es una plataforma catalana de fact-checking sin ánimo de lucro. Se dedica a verificar el discurso político y el contenido que circula en las redes y a la educación para el consumo crítico de la información. Forma parte de la International Fact-Checking Network (IFCN) y la European Fact-Checking Standards Network (EFCSN)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>La Razón</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C60" s="5" t="inlineStr">
+        <is>
+          <t>China acusa a EE UU  de "acelerar un escenario bélico" por vender armas a Taiwán</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Geopolítica</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Negativa</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>2025-12-25T11:47:46+01:00</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Las declaraciones se producen en un contexto de fricción creciente entre Pekín y Washington, en un momento en el que Estados Unidos ha reforzado su apoyo político y militar a Taipéi</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Las declaraciones se producen en un contexto de fricción creciente entre Pekín y Washington, en un momento en el que Estados Unidos ha reforzado su apoyo político y militar a Taipéi</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>La Razón</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>Empresa textil china invierte 130 millones de euros en una nueva fábrica en Fez</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Positiva</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>2025-12-25T13:10:33+01:00</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Incluye el suministro de hilados y telas, teñido, la estampación textil y la fabricación de prendas de vestir prêt-à-porter.</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Incluye el suministro de hilados y telas, teñido, la estampación textil y la fabricación de prendas de vestir prêt-à-porter.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>La Razón</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="C62" s="5" t="inlineStr">
+        <is>
+          <t>El dominio chino del juguete en la UE: dos décadas acaparando casi el 80% del mercado</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>2025-12-25T10:53:24+01:00</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>En 2024, la UE importó casi 7.072 millones de euros en juguetes procedentes del resto del mundo, de los que 5.649 millones correspondieron a China</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>En 2024, la UE importó casi 7.072 millones de euros en juguetes procedentes del resto del mundo, de los que 5.649 millones correspondieron a China</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C63" s="5" t="inlineStr">
+        <is>
+          <t>“十四五”时期信息化发展成就及电子政务发展报告发布活动在京举行</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Tecnología industrial</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2025-12-26T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>12月25日，“十四五”时期信息化发展成就及电子政务发展报告发布活动在京举行。中央网信办信息化发展局负责同志介绍了“十四五”时期我国信息化发展成就和《国家电子政务发展报告（2014—2024年）》主要内容。 “十四五”时期，在习近平新时代中国特色社会主义思想特别是习近平总书记关于网络强国的重要思想的科学指引下，中央网信办会同各地区、各有关部门认真贯彻落实党中央、国务院决策部署，扎实推进《“十四五”国家信息化规划》实施，主要目标任务顺利完成，信息化发展取得显著成就，加快从重点领域突破迈向全面赋能发展。主要体现在：信息技术创新能力显著增强，高水平自立自强步伐更加坚实；网信产业生态加快建设，以信息化培育新动能更加强劲；信息基础设施跨越式发展，经济社会信息“大动脉”更加通畅；数据资源开发利用提质增效，数据要素价值释放更加充分；信息化应用水平大幅提升，人民群众获得感、幸福感、安全感更加充足；互联网国际交流合作深入拓展，网络空间命运共同体理念更加深入人心；信息化制度机制持续健全，协同推进工作格局更加完善。 现代化建设，信息化先行。党的二十届四中全会提出信息化取得重大进展的战略目标。“十五五”时期是我国信息化发展夯实基础、全面发力的关键时期，要深入贯彻落实党中央决策部署，聚焦高质量发展主题，坚持规划引领，统筹推动国家信息化发展；坚持自立自强，大力推进网络信息技术创新；坚持融合发展，培育壮大网信产业生态；坚持夯基固本，建设完善信息基础设施；坚持普惠共享，持续提升信息化应用水平；坚持规范有序，健全完善信息化法规标准，推动我国信息化发展水平再上新台阶。 活动发布了《国家电子政务发展报告（2014—2024年）》，系统总结2014年至2024年我国电子政务发展成效和经验，分析面临形势与挑战，提出下一步重点任务，为“十五五”时期推进国家电子政务高质量发展凝聚共识、提供指引。 中央网信办网络安全协调局负责同志介绍了筑牢网络安全屏障、以高水平安全保障高质量发展有关情况。工业和信息化部信息技术发展司、国家市场监督管理总局标准技术管理司、国家数据局数据资源司以及重庆市委网信办负责同志，围绕部门和地区推动信息化发展工作介绍了有关情况。相关研究机构专家学者、媒体单位代表和网信企业代表参加了发布活动。 【责任编辑：高琳琳】</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>12月25日，“十四五”时期信息化发展成就及电子政务发展报告发布活动在京举行。中央网信办信息化发展局负责同志介绍了“十四五”时期我国信息化发展成就和《国家电子政务发展报告（2014—2024年）》主要内容。 “十四五”时期，在习近平新时代中国特色社会主义思想特别是习近平总书记关于网络强国的重要思想的科学指引下，中央网信办会同各地区、各有关部门认真贯彻落实党中央、国务院决策部署，扎实推进《“十四五”国家信息化规划》实施，主要目标任务顺利完成，信息化发展取得显著成就，加快从重点领域突破迈向全面赋能发展。主要体现在：信息技术创新能力显著增强，高水平自立自强步伐更加坚实；网信产业生态加快建设，以信息化培育新动能更加强劲；信息基础设施跨越式发展，经济社会信息“大动脉”更加通畅；数据资源开发利用提质增效，数据要素价值释放更加充分；信息化应用水平大幅提升，人民群众获得感、幸福感、安全感更加充足；互联网国际交流合作深入拓展，网络空间命运共同体理念更加深入人心；信息化制度机制持续健全，协同推进工作格局更加完善。 现代化建设，信息化先行。党的二十届四中全会提出信息化取得重大进展的战略目标。“十五五”时期是我国信息化发展夯实基础、全面发力的关键时期，要深入贯彻落实党中央决策部署，聚焦高质量发展主题，坚持规划引领，统筹推动国家信息化发展；坚持自立自强，大力推进网络信息技术创新；坚持融合发展，培育壮大网信产业生态；坚持夯基固本，建设完善信息基础设施；坚持普惠共享，持续提升信息化应用水平；坚持规范有序，健全完善信息化法规标准，推动我国信息化发展水平再上新台阶。 活动发布了《国家电子政务发展报告（2014—2024年）》，系统总结2014年至2024年我国电子政务发展成效和经验，分析面临形势与挑战，提出下一步重点任务，为“十五五”时期推进国家电子政务高质量发展凝聚共识、提供指引。 中央网信办网络安全协调局负责同志介绍了筑牢网络安全屏障、以高水平安全保障高质量发展有关情况。工业和信息化部信息技术发展司、国家市场监督管理总局标准技术管理司、国家数据局数据资源司以及重庆市委网信办负责同志，围绕部门和地区推动信息化发展工作介绍了有关情况。相关研究机构专家学者、媒体单位代表和网信企业代表参加了发布活动。 【责任编辑：高琳琳】</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C64" s="5" t="inlineStr">
+        <is>
+          <t>一图速览丨“十四五”我国信息化发展成就</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Tecnología industrial</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2025-12-26T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>【责任编辑：高琳琳】</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>【责任编辑：高琳琳】</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
+        <is>
+          <t>“智能经济”势如破竹  为经济注入“智慧芯”</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>2025-12-25T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>编者按： 韧性，是读懂2025年中国经济的关键词。宏观承压之下，一系列“新消费”现象展现出澎湃的内需活力。赛事经济、旅游经济点燃线下“烟火气”，智能经济扎实构筑产业根基；陪伴经济与情绪经济的兴起，则回应着时代的心灵需求。它们不仅是经济增长亮点，更共同勾勒出一个有温度、有弹性、面向未来的中国经济生态。 2025年9月6日，在重庆举行的2025世界智能产业博览会上，生活家居机器人与观众握手。新华社记者 陈诚 摄 ——2025新经济新现象年度盘点之三 □吕金艺 年初，穿着小花袄、挥着红手绢、扭着大秧歌的人形机器人惊艳亮相龙年春晚舞台，这不仅是中国科创力量的一次亮眼展示，更是智能经济浪潮奔涌而来的生动注脚。当机器人从实验室走向生产生活，当智能技术从单点突破迈向全域赋能，中国智能制造正以破竹之势重构产业格局，智能经济已成为驱动中国经济高质量发展的核心引擎，让奋进中国的发展春潮愈发澎湃。 智能经济的核心底气，在于国家战略引领下智能制造的深度扎根。不同于传统制造的规模化复制，智能制造以“数据+算力+算法”为核心，实现从自动化到智能化的质变，这是中国制造业由大变强的必由之路。从政策层面锚定发展方向，到企业层面深耕技术应用，我国已构建起“顶层设计+基层实践”的双轮驱动模式，让智能技术真正融入产业肌理。智能制造不是简单的机器换人，而是通过人机协同重塑生产逻辑，让生产要素实现最优配置，让产业链供应链更具韧性，这正是中国经济在变局中站稳脚跟的关键支撑。 智能经济的蓬勃生机，藏在千行百业的场景革新里。低空经济从概念走向现实，不再是单一的无人机飞行，而是智能技术赋能下的立体经济新形态，从应急救援的精准驰援到城市物流的高效配送，从低空旅游的沉浸体验到生态巡检的科技守护，低空经济以“天空赋能地面”的模式，打开了经济增长的新空间，成为新质生产力的典型代表。智能汽车超越交通工具的属性，化身移动智能终端，以自动驾驶、车路协同让出行更安全高效，更带动芯片、软件、通信等全产业链升级，构建起万亿级智能出行生态。无人酒店以无感服务重构消费体验，从入住到退房全程智能响应，背后是智能感知、大数据分析的深度应用，彰显服务业智能化转型的无限可能。智能高铁更是中国智造的标杆，智能调度让运行更精准，智能运维让安全更有保障，智能服务让旅途更舒心，铁路12306平台将铁路网与互联网相连，实现客票电子化，旅客刷脸、刷身份证即可进站乘车，智能服务让智能化出行轻松便捷，同时也为沿线的人们打开了财富密码，以“智能+交通”的融合，书写大国重器的新传奇。这些场景的迭代，本质是智能经济对生产生活方式的重构，让效率与体验实现双重提升。 智能经济的独特优势，在于中国优越的发展土壤与内生动力。我国拥有超大规模市场，为智能技术提供了天然试验场，需求牵引技术迭代，技术反哺需求升级，形成良性循环；完备的产业体系让智能技术从研发到落地无缝衔接，避免“卡脖子”困境；海量的数据资源更是智能经济的核心生产要素，为算法优化、模型训练提供充足养分。不同于西方部分国家的技术垄断思维，中国智能经济走的是开放融合之路，既深耕核心技术自主创新，又推动跨界协同发展，“智能+制造”“智能+服务”“智能+农业”的多元融合，让智能经济的辐射力持续增强，带动全产业链提质增效。 从智能经济看中国经济未来，光明前景清晰可见。智能经济让中国经济增长更具内生动力，摆脱传统路径依赖，以技术创新驱动高质量发展，破解“规模红利消退”的难题；让中国经济结构更趋优化，传统产业焕新升级，新兴产业蓬勃生长，形成多点支撑、多极发力的产业格局；让中国经济更具全球竞争力，在人工智能、智能制造等关键领域抢占先机，为参与全球经济治理注入中国力量。智能经济不是简单的技术叠加，而是发展理念的革新，是发展模式的升级，它让中国经济在时代浪潮中找准航向，在攻坚克难中积蓄力量。 春潮涌动处，扬帆奋进时。人形机器人的灵动身影，低空经济的广阔天地，智能汽车的驰骋向前，智能高铁的追风逐梦，都是智能经济赋能中国发展的生动缩影。智能经济势如破竹，不仅重塑着当下的产业图景，更擘画着中国经济的未来模样。只要锚定创新方向，深耕智能赛道，以实干笃定前行，以创新破局开路，奋进中国必将在智能经济的浪潮中乘风破浪，书写更加璀璨的发展篇章，让中国经济的春潮奔涌不息，奔向更加光明的远方。 （中国互联网发展基金会中国正能量网络传播专项基金支持项目） 【责任编辑：曹静】</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>编者按： 韧性，是读懂2025年中国经济的关键词。宏观承压之下，一系列“新消费”现象展现出澎湃的内需活力。赛事经济、旅游经济点燃线下“烟火气”，智能经济扎实构筑产业根基；陪伴经济与情绪经济的兴起，则回应着时代的心灵需求。它们不仅是经济增长亮点，更共同勾勒出一个有温度、有弹性、面向未来的中国经济生态。 2025年9月6日，在重庆举行的2025世界智能产业博览会上，生活家居机器人与观众握手。新华社记者 陈诚 摄 ——2025新经济新现象年度盘点之三 □吕金艺 年初，穿着小花袄、挥着红手绢、扭着大秧歌的人形机器人惊艳亮相龙年春晚舞台，这不仅是中国科创力量的一次亮眼展示，更是智能经济浪潮奔涌而来的生动注脚。当机器人从实验室走向生产生活，当智能技术从单点突破迈向全域赋能，中国智能制造正以破竹之势重构产业格局，智能经济已成为驱动中国经济高质量发展的核心引擎，让奋进中国的发展春潮愈发澎湃。 智能经济的核心底气，在于国家战略引领下智能制造的深度扎根。不同于传统制造的规模化复制，智能制造以“数据+算力+算法”为核心，实现从自动化到智能化的质变，这是中国制造业由大变强的必由之路。从政策层面锚定发展方向，到企业层面深耕技术应用，我国已构建起“顶层设计+基层实践”的双轮驱动模式，让智能技术真正融入产业肌理。智能制造不是简单的机器换人，而是通过人机协同重塑生产逻辑，让生产要素实现最优配置，让产业链供应链更具韧性，这正是中国经济在变局中站稳脚跟的关键支撑。 智能经济的蓬勃生机，藏在千行百业的场景革新里。低空经济从概念走向现实，不再是单一的无人机飞行，而是智能技术赋能下的立体经济新形态，从应急救援的精准驰援到城市物流的高效配送，从低空旅游的沉浸体验到生态巡检的科技守护，低空经济以“天空赋能地面”的模式，打开了经济增长的新空间，成为新质生产力的典型代表。智能汽车超越交通工具的属性，化身移动智能终端，以自动驾驶、车路协同让出行更安全高效，更带动芯片、软件、通信等全产业链升级，构建起万亿级智能出行生态。无人酒店以无感服务重构消费体验，从入住到退房全程智能响应，背后是智能感知、大数据分析的深度应用，彰显服务业智能化转型的无限可能。智能高铁更是中国智造的标杆，智能调度让运行更精准，智能运维让安全更有保障，智能服务让旅途更舒心，铁路12306平台将铁路网与互联网相连，实现客票电子化，旅客刷脸、刷身份证即可进站乘车，智能服务让智能化出行轻松便捷，同时也为沿线的人们打开了财富密码，以“智能+交通”的融合，书写大国重器的新传奇。这些场景的迭代，本质是智能经济对生产生活方式的重构，让效率与体验实现双重提升。 智能经济的独特优势，在于中国优越的发展土壤与内生动力。我国拥有超大规模市场，为智能技术提供了天然试验场，需求牵引技术迭代，技术反哺需求升级，形成良性循环；完备的产业体系让智能技术从研发到落地无缝衔接，避免“卡脖子”困境；海量的数据资源更是智能经济的核心生产要素，为算法优化、模型训练提供充足养分。不同于西方部分国家的技术垄断思维，中国智能经济走的是开放融合之路，既深耕核心技术自主创新，又推动跨界协同发展，“智能+制造”“智能+服务”“智能+农业”的多元融合，让智能经济的辐射力持续增强，带动全产业链提质增效。 从智能经济看中国经济未来，光明前景清晰可见。智能经济让中国经济增长更具内生动力，摆脱传统路径依赖，以技术创新驱动高质量发展，破解“规模红利消退”的难题；让中国经济结构更趋优化，传统产业焕新升级，新兴产业蓬勃生长，形成多点支撑、多极发力的产业格局；让中国经济更具全球竞争力，在人工智能、智能制造等关键领域抢占先机，为参与全球经济治理注入中国力量。智能经济不是简单的技术叠加，而是发展理念的革新，是发展模式的升级，它让中国经济在时代浪潮中找准航向，在攻坚克难中积蓄力量。 春潮涌动处，扬帆奋进时。人形机器人的灵动身影，低空经济的广阔天地，智能汽车的驰骋向前，智能高铁的追风逐梦，都是智能经济赋能中国发展的生动缩影。智能经济势如破竹，不仅重塑着当下的产业图景，更擘画着中国经济的未来模样。只要锚定创新方向，深耕智能赛道，以实干笃定前行，以创新破局开路，奋进中国必将在智能经济的浪潮中乘风破浪，书写更加璀璨的发展篇章，让中国经济的春潮奔涌不息，奔向更加光明的远方。 （中国互联网发展基金会中国正能量网络传播专项基金支持项目） 【责任编辑：曹静】</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C66" s="5" t="inlineStr">
+        <is>
+          <t>“十四五”时期我国信息化成果显著</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Tecnología industrial</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>2025-12-25T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>今天（25日），中央网信办、工业和信息化部、国家市场监督管理总局、国家数据局等部门联合召开发布会，中央网信办相关负责人介绍，“十四五”期间，我国网络信息技术创新取得新突破，信息基础设施实现新跨越，信息化应用水平实现新提升，加快从重点领域突破迈向全面赋能发展。 据中央网信办相关负责人介绍，“十四五”期间，我国信息技术创新能力显著增强，高水平自立自强步伐更加坚实。五年来，我国坚持把创新作为信息化发展的第一动力，形成一批标志性、原创性、颠覆性科技创新成果。 中央网信办信息化发展局局长 温锐松：集成电路、人工智能、基础软件等领域取得新成果，搭载开源鸿蒙操作系统的产品总量超11.9亿台，通义千问、DeepSeek等多款产品性能位于全球前列，超700款生成式人工智能大模型产品完成备案，具身智能逐步走向产业应用，智能体加速创新发展。 温锐松介绍，“十四五”期间我国信息化领域除了关键核心技术加速突破，前沿信息技术也在加快布局。6G技术研发和标准研制扎实推进，已完成第一阶段技术试验，形成超过300项关键技术储备。 网信产业生态加快建设 以信息化培育新动能更加强劲 五年来，我国信息化发展坚持补短板、拉长板、锻新板，构建网信产业体系，推进数智技术赋能实体经济。网信产业生态加快建设，以信息化培育新动能更加强劲。 “十四五”期间，我国数字经济核心产业增加值占GDP比重从7.8%增至10.4%，数字经济规模稳居世界第二。2024年规模以上电子信息制造业营业收入达16.19万亿元，软件业务收入达13.73万亿元，分别较“十三五”末提升33.8%和68.2%。 赋能传统产业转型升级成效明显，制造业数字化转型提速扩面，重点工业企业数字化研发设计工具普及率从73%提升至85.4%，关键工序数控化率从52.1%提升至68.5%，全国网上零售额从11.76万亿元提升至15.23万亿元，稳居全球最大网络零售市场。 中央网信办信息化发展局局长 温锐松：数字化绿色化协同转型发展提速增效，钢铁行业数字化能碳管理已覆盖全国40%产能，绿色低碳数字生产生活方式更加普及。网信企业活力不断增强，我国高新技术企业突破50万家，网信企业创新能力不断提升。 我国数据资源开发利用提质增效 5年来，我国数据资源开发利用提质增效，年度数据生产量从2022年的26.83ZB增长至2024年的41.06ZB，占全球数据总量26.67%。另外，我国信息化应用水平大幅提升，建成全国政务服务“一张网”，92.5%的省级行政许可事项实现网上受理和“最多跑一次”。 数据基础制度初步建立，《中共中央 国务院关于构建数据基础制度更好发挥数据要素作用的意见》印发实施，配套政策措施陆续出台。我国年度数据生产量从2022年的26.83ZB增长至2024年的41.06ZB，占全球数据总量26.67%。建成国家公共数据资源登记平台，深入实施“数据要素×”行动，涌现一批典型应用场景和案例。 中央网信办信息化发展局局长 温锐松：电子政务发展稳步前行，建成全国政务服务“一张网”，92.5%的省级行政许可事项实现网上受理和“最多跑一次”，推动更多事项从“能办”“好办”转为“高效办成”。“十四五”时期，我国网民规模从9.89亿人增长至11.23亿人，互联网普及率从70.4%提升至79.7%，六成以上公民具备初级及以上数字素养与技能，信息化促进教育、医疗、文化等优质资源普及下沉。 5年来，我国数字乡村发展成效明显，部署开展两批国家数字乡村试点，实施数字乡村强农惠农富农专项行动，“十四五”期间我国城乡互联网普及率差距较“十三五”末缩小8.2个百分点，农业生产信息化率从22.5%增至30%以上，全国农村网络零售额超2.5万亿元，较“十三五”末增长43%，远程医疗服务网络覆盖全国所有市县，城乡数字鸿沟加快弥合。 （总台央视记者 李本扬 张岗 范月鸣 张喆） 【责任编辑：曹静】</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>今天（25日），中央网信办、工业和信息化部、国家市场监督管理总局、国家数据局等部门联合召开发布会，中央网信办相关负责人介绍，“十四五”期间，我国网络信息技术创新取得新突破，信息基础设施实现新跨越，信息化应用水平实现新提升，加快从重点领域突破迈向全面赋能发展。 据中央网信办相关负责人介绍，“十四五”期间，我国信息技术创新能力显著增强，高水平自立自强步伐更加坚实。五年来，我国坚持把创新作为信息化发展的第一动力，形成一批标志性、原创性、颠覆性科技创新成果。 中央网信办信息化发展局局长 温锐松：集成电路、人工智能、基础软件等领域取得新成果，搭载开源鸿蒙操作系统的产品总量超11.9亿台，通义千问、DeepSeek等多款产品性能位于全球前列，超700款生成式人工智能大模型产品完成备案，具身智能逐步走向产业应用，智能体加速创新发展。 温锐松介绍，“十四五”期间我国信息化领域除了关键核心技术加速突破，前沿信息技术也在加快布局。6G技术研发和标准研制扎实推进，已完成第一阶段技术试验，形成超过300项关键技术储备。 网信产业生态加快建设 以信息化培育新动能更加强劲 五年来，我国信息化发展坚持补短板、拉长板、锻新板，构建网信产业体系，推进数智技术赋能实体经济。网信产业生态加快建设，以信息化培育新动能更加强劲。 “十四五”期间，我国数字经济核心产业增加值占GDP比重从7.8%增至10.4%，数字经济规模稳居世界第二。2024年规模以上电子信息制造业营业收入达16.19万亿元，软件业务收入达13.73万亿元，分别较“十三五”末提升33.8%和68.2%。 赋能传统产业转型升级成效明显，制造业数字化转型提速扩面，重点工业企业数字化研发设计工具普及率从73%提升至85.4%，关键工序数控化率从52.1%提升至68.5%，全国网上零售额从11.76万亿元提升至15.23万亿元，稳居全球最大网络零售市场。 中央网信办信息化发展局局长 温锐松：数字化绿色化协同转型发展提速增效，钢铁行业数字化能碳管理已覆盖全国40%产能，绿色低碳数字生产生活方式更加普及。网信企业活力不断增强，我国高新技术企业突破50万家，网信企业创新能力不断提升。 我国数据资源开发利用提质增效 5年来，我国数据资源开发利用提质增效，年度数据生产量从2022年的26.83ZB增长至2024年的41.06ZB，占全球数据总量26.67%。另外，我国信息化应用水平大幅提升，建成全国政务服务“一张网”，92.5%的省级行政许可事项实现网上受理和“最多跑一次”。 数据基础制度初步建立，《中共中央 国务院关于构建数据基础制度更好发挥数据要素作用的意见》印发实施，配套政策措施陆续出台。我国年度数据生产量从2022年的26.83ZB增长至2024年的41.06ZB，占全球数据总量26.67%。建成国家公共数据资源登记平台，深入实施“数据要素×”行动，涌现一批典型应用场景和案例。 中央网信办信息化发展局局长 温锐松：电子政务发展稳步前行，建成全国政务服务“一张网”，92.5%的省级行政许可事项实现网上受理和“最多跑一次”，推动更多事项从“能办”“好办”转为“高效办成”。“十四五”时期，我国网民规模从9.89亿人增长至11.23亿人，互联网普及率从70.4%提升至79.7%，六成以上公民具备初级及以上数字素养与技能，信息化促进教育、医疗、文化等优质资源普及下沉。 5年来，我国数字乡村发展成效明显，部署开展两批国家数字乡村试点，实施数字乡村强农惠农富农专项行动，“十四五”期间我国城乡互联网普及率差距较“十三五”末缩小8.2个百分点，农业生产信息化率从22.5%增至30%以上，全国农村网络零售额超2.5万亿元，较“十三五”末增长43%，远程医疗服务网络覆盖全国所有市县，城乡数字鸿沟加快弥合。 （总台央视记者 李本扬 张岗 范月鸣 张喆） 【责任编辑：曹静】</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C67" s="5" t="inlineStr">
+        <is>
+          <t>体育育出消费新引擎</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Muy positiva</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>2025-12-25T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>新华社北京12月24日电题：体育育出消费新引擎——“体育深化改革新气象”组稿之二 新华社记者王恒志、王春燕、岳冉冉 “苏超”带动民间足球热潮，冰雪产业规模将突破万亿元，粤港澳全运会精彩纷呈……2025年，中国体育经济呈现加速发展态势。这得益于过去几年里，促进体育经济发展的政策文件密集出台，体育赛事“三进”活动广泛开展，“跟着赛事去旅行”深入人心，产业发展平台建设初见成效。与此同时，各地持续探索创新举措，推动有效市场与有为政府深度融合，让中国体育经济迸发出巨大能量，为扩大内需、提振消费提供了更加丰富的优质商品和服务供给。 12月6日，滑雪爱好者在黑龙江省亚布力滑雪旅游度假区雪场体验滑雪（无人机照片）。新华社发（原勇摄） 政策研制铺就发展快车道 2025新疆热雪节、第29届长春冰雪节、河北承德冰雪温泉旅游季、第21届内蒙古自治区冰雪那达慕、第22届中国·满洲里中俄蒙国际冰雪节、重庆冰雪运动季……又是一年冰雪季，不仅东北、内蒙古、新疆等地因地制宜打造特色品牌，南方一些具备条件的地方也积极布局冰雪产业。 《中国冰雪产业发展研究报告（2025）》显示，2025年我国冰雪产业规模将突破万亿元。从北方到全国、从冬季到四季，冰雪经济正创建消费新场景、打造产业新生态、带来区域发展新机遇。 冰雪经济蓬勃发展，离不开政策加力支持。2024年11月，国务院办公厅印发《关于以冰雪运动高质量发展激发冰雪经济活力的若干意见》，推动冰雪运动、冰雪文化、冰雪装备、冰雪旅游全产业链发展。中共中央办公厅、国务院办公厅印发的《提振消费专项行动方案》提出要推动冰雪消费，启动实施冰雪旅游提升计划，组织开展冰雪消费季等促消费活动，鼓励各地因时因地丰富冰雪场地和消费产品供给。今年政府工作报告也提出，要积极发展冰雪运动和冰雪经济。一系列政策举措为冰雪经济发展提供了重要指引。 12月18日，参观者在第九届吉林冰雪产业国际博览会现场参观展出的国产碳纤维滑雪板。新华社记者 许畅 摄 冰雪经济的迅猛发展，是近年来中国体育产业借助政策支持加快发展的生动缩影。2025年9月，国务院办公厅印发的《关于释放体育消费潜力进一步推进体育产业高质量发展的意见》明确提出，到2030年，培育一批具有世界影响力的体育企业和体育赛事，体育产业发展水平大幅跃升，总规模超过7万亿元，在构建新发展格局中发挥重要作用。 近两年中国户外运动发展迅猛，同样得益于政策引导。2025年1月，国务院办公厅转发国家发展改革委、体育总局《关于建设高质量户外运动目的地的指导意见》，各地纷纷因地制宜，探索适合自身禀赋的户外运动目的地建设路径。 此外，国家体育总局还大力推动体育标准化建设，加强体育标准化顶层设计，逐渐构建起宏观引领、专项支撑、部门协同的政策矩阵，有力促进体育产业健康快速发展。 5月17日，参赛者在2025黄浦江源第二届全国山地户外运动挑战赛中。新华社记者 黄宗治 摄 体育赛事经济亮点频现 “苏超”如火如荼、中超上座人次创新高、全运会“大湾鸡”走红网络……2025年虽然没有奥运会、世界杯这样的国际顶级赛事，却堪称中国体育赛事经济“大年”。国家体育总局坚持以赛事体系建设为核心，“赛事+”“+赛事”深度融合，形成“一体两翼”发展思路，着力推动赛事经济发展，不断丰富大型体育赛事、职业赛事、群众赛事活动供给。 从全运盛会到民间赛事，从职业体育到业余足球，国家体育总局会同商务部、文化和旅游部开展的“体育赛事进景区、进街区、进商圈”“跟着赛事去旅行”“乐享精彩赛事 寻味中华美食”等活动，激发全民参与热情，提振消费效应持续显现。 国家体育总局还创新开展促进体育消费和赛事经济试点，在全国选取30个城市，鼓励试点单位创新政策措施。江苏省无锡市作为首批试点城市，举办了无锡马拉松、世界跆拳道大满贯系列赛事、亚洲体育舞蹈节、阳羡100越野挑战赛等自有IP赛事，并承办各类高水平国际国内赛事。其中，仅2025无锡马拉松就吸引39.1万人现场观赛，拉动餐饮、住宿、交通、旅游、展会等经济效益5.05亿元、同比增长78.2%。目前，国家体育总局正在进一步规范马拉松赛事组织工作，让赛事更好地服务于地方经济社会发展。 图为10月30日在江苏无锡举行的一场2025年世界跆拳道锦标赛比赛。新华社发（刘臻睿摄） 如今，“跟着赛事去旅行”在各地广泛开展。“体育赛事进景区、进街区、进商圈”让不少以往受众有限的赛事走到百姓身边。2025赛季中国男子三人篮球超级联赛（简称“超三联赛”）常规赛设置25站大区赛、4站争霸赛，其中11站赛事走进城市核心商圈，成为激活城市空间、促进体育消费的新引擎。在北京西城区，“超三联赛”的一张赛事票根可享40多个品牌优惠，推出“亲子游”“休闲派”两条特色打卡路线，串联起20余个文商旅体重点点位。在江苏省张家港市，金茂览秀城商圈赛事期间客流量达15.36万人次，同比提升6%，销售额提升10%，达1252万元。 国家体育总局在河北、江苏、浙江等地开展赛事活动带动消费的监测试点。监测结果显示，2025年上半年，7个试点省份监测的511场重点赛事活动，带动体育及相关消费超160亿元，场均带动超3000万元。 创新搭建产业发展平台 2023年首届中国户外运动产业大会在大理举办时，云南省就明确了“全域布局、特色发展”的路径。云南省体育局局长杨中华说：“大会落户云南三年来，我们以户外运动破局体育产业发展，推动体育及相关产业规模三年实现翻番，年均增长23%，2025年将突破千亿元大关。户外运动正成为云南经济增长新引擎。” 图为10月24日拍摄的2025中国户外运动产业大会开幕式现场。新华社记者 胡超 摄 户外运动正成为中国体育经济新的增长点。国家体育总局体育经济司发布的《中国户外运动产业发展报告（2024-2025）》显示，截至2025年6月底，我国户外运动相关企业已达33.5万家，其中，2025年上半年新增注册相关企业2.4万余家。与此同时，截至2025年4月初，我国户外运动参与人数已突破4亿人。 近年来，国家体育总局持续加强产业发展平台建设，中国户外运动产业大会正是着力打造的重要平台之一，其目标就是整合户外运动资源，聚焦行业发展趋势，持续培育新产品、新服务、新业态。此外，还连续多年举办中国国际体育用品博览会、中国体育旅游博览会等展会，搭建产需对接平台，并在服贸会连续多年设置体育服务专题，在进博会设置体育用品及赛事专区。 【责任编辑：曹静】</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>新华社北京12月24日电题：体育育出消费新引擎——“体育深化改革新气象”组稿之二 新华社记者王恒志、王春燕、岳冉冉 “苏超”带动民间足球热潮，冰雪产业规模将突破万亿元，粤港澳全运会精彩纷呈……2025年，中国体育经济呈现加速发展态势。这得益于过去几年里，促进体育经济发展的政策文件密集出台，体育赛事“三进”活动广泛开展，“跟着赛事去旅行”深入人心，产业发展平台建设初见成效。与此同时，各地持续探索创新举措，推动有效市场与有为政府深度融合，让中国体育经济迸发出巨大能量，为扩大内需、提振消费提供了更加丰富的优质商品和服务供给。 12月6日，滑雪爱好者在黑龙江省亚布力滑雪旅游度假区雪场体验滑雪（无人机照片）。新华社发（原勇摄） 政策研制铺就发展快车道 2025新疆热雪节、第29届长春冰雪节、河北承德冰雪温泉旅游季、第21届内蒙古自治区冰雪那达慕、第22届中国·满洲里中俄蒙国际冰雪节、重庆冰雪运动季……又是一年冰雪季，不仅东北、内蒙古、新疆等地因地制宜打造特色品牌，南方一些具备条件的地方也积极布局冰雪产业。 《中国冰雪产业发展研究报告（2025）》显示，2025年我国冰雪产业规模将突破万亿元。从北方到全国、从冬季到四季，冰雪经济正创建消费新场景、打造产业新生态、带来区域发展新机遇。 冰雪经济蓬勃发展，离不开政策加力支持。2024年11月，国务院办公厅印发《关于以冰雪运动高质量发展激发冰雪经济活力的若干意见》，推动冰雪运动、冰雪文化、冰雪装备、冰雪旅游全产业链发展。中共中央办公厅、国务院办公厅印发的《提振消费专项行动方案》提出要推动冰雪消费，启动实施冰雪旅游提升计划，组织开展冰雪消费季等促消费活动，鼓励各地因时因地丰富冰雪场地和消费产品供给。今年政府工作报告也提出，要积极发展冰雪运动和冰雪经济。一系列政策举措为冰雪经济发展提供了重要指引。 12月18日，参观者在第九届吉林冰雪产业国际博览会现场参观展出的国产碳纤维滑雪板。新华社记者 许畅 摄 冰雪经济的迅猛发展，是近年来中国体育产业借助政策支持加快发展的生动缩影。2025年9月，国务院办公厅印发的《关于释放体育消费潜力进一步推进体育产业高质量发展的意见》明确提出，到2030年，培育一批具有世界影响力的体育企业和体育赛事，体育产业发展水平大幅跃升，总规模超过7万亿元，在构建新发展格局中发挥重要作用。 近两年中国户外运动发展迅猛，同样得益于政策引导。2025年1月，国务院办公厅转发国家发展改革委、体育总局《关于建设高质量户外运动目的地的指导意见》，各地纷纷因地制宜，探索适合自身禀赋的户外运动目的地建设路径。 此外，国家体育总局还大力推动体育标准化建设，加强体育标准化顶层设计，逐渐构建起宏观引领、专项支撑、部门协同的政策矩阵，有力促进体育产业健康快速发展。 5月17日，参赛者在2025黄浦江源第二届全国山地户外运动挑战赛中。新华社记者 黄宗治 摄 体育赛事经济亮点频现 “苏超”如火如荼、中超上座人次创新高、全运会“大湾鸡”走红网络……2025年虽然没有奥运会、世界杯这样的国际顶级赛事，却堪称中国体育赛事经济“大年”。国家体育总局坚持以赛事体系建设为核心，“赛事+”“+赛事”深度融合，形成“一体两翼”发展思路，着力推动赛事经济发展，不断丰富大型体育赛事、职业赛事、群众赛事活动供给。 从全运盛会到民间赛事，从职业体育到业余足球，国家体育总局会同商务部、文化和旅游部开展的“体育赛事进景区、进街区、进商圈”“跟着赛事去旅行”“乐享精彩赛事 寻味中华美食”等活动，激发全民参与热情，提振消费效应持续显现。 国家体育总局还创新开展促进体育消费和赛事经济试点，在全国选取30个城市，鼓励试点单位创新政策措施。江苏省无锡市作为首批试点城市，举办了无锡马拉松、世界跆拳道大满贯系列赛事、亚洲体育舞蹈节、阳羡100越野挑战赛等自有IP赛事，并承办各类高水平国际国内赛事。其中，仅2025无锡马拉松就吸引39.1万人现场观赛，拉动餐饮、住宿、交通、旅游、展会等经济效益5.05亿元、同比增长78.2%。目前，国家体育总局正在进一步规范马拉松赛事组织工作，让赛事更好地服务于地方经济社会发展。 图为10月30日在江苏无锡举行的一场2025年世界跆拳道锦标赛比赛。新华社发（刘臻睿摄） 如今，“跟着赛事去旅行”在各地广泛开展。“体育赛事进景区、进街区、进商圈”让不少以往受众有限的赛事走到百姓身边。2025赛季中国男子三人篮球超级联赛（简称“超三联赛”）常规赛设置25站大区赛、4站争霸赛，其中11站赛事走进城市核心商圈，成为激活城市空间、促进体育消费的新引擎。在北京西城区，“超三联赛”的一张赛事票根可享40多个品牌优惠，推出“亲子游”“休闲派”两条特色打卡路线，串联起20余个文商旅体重点点位。在江苏省张家港市，金茂览秀城商圈赛事期间客流量达15.36万人次，同比提升6%，销售额提升10%，达1252万元。 国家体育总局在河北、江苏、浙江等地开展赛事活动带动消费的监测试点。监测结果显示，2025年上半年，7个试点省份监测的511场重点赛事活动，带动体育及相关消费超160亿元，场均带动超3000万元。 创新搭建产业发展平台 2023年首届中国户外运动产业大会在大理举办时，云南省就明确了“全域布局、特色发展”的路径。云南省体育局局长杨中华说：“大会落户云南三年来，我们以户外运动破局体育产业发展，推动体育及相关产业规模三年实现翻番，年均增长23%，2025年将突破千亿元大关。户外运动正成为云南经济增长新引擎。” 图为10月24日拍摄的2025中国户外运动产业大会开幕式现场。新华社记者 胡超 摄 户外运动正成为中国体育经济新的增长点。国家体育总局体育经济司发布的《中国户外运动产业发展报告（2024-2025）》显示，截至2025年6月底，我国户外运动相关企业已达33.5万家，其中，2025年上半年新增注册相关企业2.4万余家。与此同时，截至2025年4月初，我国户外运动参与人数已突破4亿人。 近年来，国家体育总局持续加强产业发展平台建设，中国户外运动产业大会正是着力打造的重要平台之一，其目标就是整合户外运动资源，聚焦行业发展趋势，持续培育新产品、新服务、新业态。此外，还连续多年举办中国国际体育用品博览会、中国体育旅游博览会等展会，搭建产需对接平台，并在服贸会连续多年设置体育服务专题，在进博会设置体育用品及赛事专区。 【责任编辑：曹静】</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>China Daily (Chinese)</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="C68" s="5" t="inlineStr">
+        <is>
+          <t>北京：调减非京籍家庭购房社保或个税缴纳年限</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Economia</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Positiva</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2025-12-24T00:00:00+00:00</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>北京市贯彻落实中央经济工作会议精神，着力稳定房地产市场。12月24日，市住房城乡建设委、市发展改革委、人民银行北京市分行、北京住房公积金管理中心等4部门联合印发《关于进一步优化调整本市房地产相关政策的通知》(以下简称《通知》)，自2025年12月24日起施行。 《通知》明确，为更好满足居民刚性住房需求和多样化改善性住房需求，进一步优化调整住房限购政策。一是放宽非京籍家庭购房条件。将非京籍家庭购买五环内商品住房的社保或个税缴纳年限，由现行的“3年”调减为“2年”；购买五环外商品住房的，由现行的“2年”调减为“1年”。二是支持多子女家庭住房需求。二孩及以上的多子女家庭，可在五环内多购买一套商品住房，即：京籍多子女家庭，可在五环内购买3套商品住房；在京连续2年缴纳社保或个税的非京籍多子女家庭，可在五环内购买2套商品住房。 《通知》明确，进一步优化个人住房信贷政策，银行业金融机构根据北京地区市场利率定价自律机制要求和本机构经营状况、客户风险状况等因素，在利率定价机制安排方面不再区分首套住房和二套住房，合理确定每笔商业性个人住房贷款的具体利率水平。关于住房贷款相关业务，可向经办银行具体咨询。 《通知》明确，加大公积金支持住房消费力度，调整二套住房公积金贷款最低首付比例，对借款申请人(含共同申请人)使用公积金个人住房贷款购买二套住房的，最低首付款比例由不低于30%调整为不低于25%。 《通知》还提出，为进一步优化营商环境，提升房地产投资效率，调整招拍挂拿地的房地产开发项目立项方式，由市区分级核准调整为区级备案。 【责任编辑：吴艳鹏】</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>北京市贯彻落实中央经济工作会议精神,着力稳定房地产市场。12月24日,市住房城乡建设委、市发展改革委、人民银行北京市分行、北京住房公积金管理中心等4部门联合印发《关于进一步优化调整本市房地产相关政策的通知》(以下简称《通知》),自2025年12月24日起施行。
+《通知》明确,为更好满足居民刚性住房需求和多样化改善性住房需求,进一步优化调整住房限购政策。一是放宽非京籍家庭购房条件。将非京籍家庭购买五环内商品住房的社保或个税缴纳年限,由现行的“3年”调减为“2年”;购买五环外商品住房的,由现行的“2年”调减为“1年”。二是支持多子女家庭住房需求。二孩及以上的多子女家庭,可在五环内多购买一套商品住房,即:京籍多子女家庭,可在五环内购买3套商品住房;在京连续2年缴纳社保或个税的非京籍多子女家庭,可在五环内购买2套商品住房。
+《通知》明确,进一步优化个人住房信贷政策,银行业金融机构根据北京地区市场利率定价自律机制要求和本机构经营状况、客户风险状况等因素,在利率定价机制安排方面不再区分首套住房和二套住房,合理确定每笔商业性个人住房贷款的具体利率水平。关于住房贷款相关业务,可向经办银行具体咨询。
+《通知》明确,加大公积金支持住房消费力度,调整二套住房公积金贷款最低首付比例,对借款申请人(含共同申请人)使用公积金个人住房贷款购买二套住房的,最低首付款比例由不低于30%调整为不低于25%。
+《通知》还提出,为进一步优化营商环境,提升房地产投资效率,调整招拍挂拿地的房地产开发项目立项方式,由市区分级核准调整为区级备案。</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId1"/>
@@ -3543,10 +4654,32 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C44" r:id="rId43"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C45" r:id="rId44"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C46" r:id="rId45"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C47" r:id="rId46"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C48" r:id="rId47"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C49" r:id="rId48"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C50" r:id="rId49"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C51" r:id="rId50"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C52" r:id="rId51"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C53" r:id="rId52"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C54" r:id="rId53"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C55" r:id="rId54"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C56" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C57" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C58" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C59" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C60" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C61" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C62" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C63" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C64" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C65" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C66" r:id="rId65"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C67" r:id="rId66"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C68" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId68"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3584,7 +4717,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>22-12-2025 18:22:21</t>
+          <t>26-12-2025 11:43:58</t>
         </is>
       </c>
     </row>

</xml_diff>